<commit_message>
Corrected missing policy ID numbers
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -490,7 +490,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5323" uniqueCount="1957">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5326" uniqueCount="1960">
   <si>
     <t>Short Name</t>
   </si>
@@ -7474,6 +7474,15 @@
       </rPr>
       <t xml:space="preserve"> https://www.ongcindia.com/wps/wcm/connect/en/sustainability/energy-center/research-projects-by-oec/</t>
     </r>
+  </si>
+  <si>
+    <t>Checks for Policy ID Number Validity</t>
+  </si>
+  <si>
+    <t>Lowest duplicate ID number</t>
+  </si>
+  <si>
+    <t>Row of first enabled policy missing a valid ID number</t>
   </si>
 </sst>
 </file>
@@ -8541,7 +8550,7 @@
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="400">
+  <cellXfs count="406">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -9582,6 +9591,9 @@
     <xf numFmtId="0" fontId="0" fillId="30" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="30" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -9594,9 +9606,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -9606,12 +9615,20 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="30" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="2x indented GHG Textfiels" xfId="10"/>
@@ -9635,7 +9652,47 @@
     <cellStyle name="Обычный_CRF2002 (1)" xfId="13"/>
     <cellStyle name="Обычный_LULUCF module - v 1.0" xfId="15"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="56">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -10702,206 +10759,251 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="16384" width="8.86328125" style="9"/>
+    <col min="1" max="1" width="28.265625" style="9" customWidth="1"/>
+    <col min="2" max="16384" width="8.86328125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:2">
       <c r="A1" s="13" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:2">
       <c r="A3" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:2">
       <c r="A4" s="9" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:2">
       <c r="A5" s="9" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:2">
       <c r="A6" s="9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:2">
       <c r="A8" s="9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:2">
       <c r="A9" s="9" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:2">
       <c r="A10" s="49" t="s">
         <v>1356</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:2">
       <c r="A11" s="49"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:2">
       <c r="A12" s="9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:2">
       <c r="A13" s="9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:2">
       <c r="A14" s="9" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:2">
       <c r="A16" s="50" t="s">
+        <v>1957</v>
+      </c>
+      <c r="B16" s="176"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="400" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B17" s="118">
+        <f>MAX(PolicyLevers!H:H)</f>
+        <v>555</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="401" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B18" s="118" t="e">
+        <f>IF(MIN(IF(COUNTIF(PolicyLevers!$H$2:$H$1500,PolicyLevers!$H$2:$H$1500)&gt;1,PolicyLevers!$H$2:$H$1500, ""))=0,"No duplicate ID numbers",MIN(IF(COUNTIF(PolicyLevers!$H$2:$H$1500,PolicyLevers!$H$2:$H$1500)&gt;1,PolicyLevers!$H$2:$H$1500, "")))</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="99.75">
+      <c r="A19" s="402" t="s">
+        <v>1959</v>
+      </c>
+      <c r="B19" s="118" t="str">
+        <f>IF(MIN(IF((NOT(ISNUMBER(PolicyLevers!$H$2:$H$1500)))*(PolicyLevers!$I$2:$I$1500="Yes"),ROW(PolicyLevers!$H$2:$H$1500)))=0,"No missing ID numbers",MIN(IF((NOT(ISNUMBER(PolicyLevers!$H$2:$H$1500)))*(PolicyLevers!$I$2:$I$1500="Yes"),ROW(PolicyLevers!$H$2:$H$1500))))</f>
+        <v>No missing ID numbers</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="50" t="s">
         <v>1452</v>
       </c>
-      <c r="B16" s="176"/>
-      <c r="C16" s="176"/>
-      <c r="D16" s="176"/>
-      <c r="E16" s="176"/>
-      <c r="F16" s="176"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="9" t="s">
+      <c r="B21" s="176"/>
+      <c r="C21" s="176"/>
+      <c r="D21" s="176"/>
+      <c r="E21" s="176"/>
+      <c r="F21" s="176"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="9" t="s">
         <v>1453</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="9" t="s">
+    <row r="23" spans="1:6">
+      <c r="A23" s="9" t="s">
         <v>1437</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="9" t="s">
+    <row r="24" spans="1:6">
+      <c r="A24" s="9" t="s">
         <v>1438</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="9" t="s">
+    <row r="25" spans="1:6">
+      <c r="A25" s="9" t="s">
         <v>1439</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="9" t="s">
+    <row r="26" spans="1:6">
+      <c r="A26" s="9" t="s">
         <v>1440</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="9" t="s">
+    <row r="28" spans="1:6">
+      <c r="A28" s="9" t="s">
         <v>1454</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="9" t="s">
+    <row r="29" spans="1:6">
+      <c r="A29" s="9" t="s">
         <v>1435</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="9" t="s">
+    <row r="30" spans="1:6">
+      <c r="A30" s="9" t="s">
         <v>1436</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="9" t="s">
+    <row r="32" spans="1:6">
+      <c r="A32" s="9" t="s">
         <v>1455</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="9" t="s">
-        <v>1442</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="9" t="s">
-        <v>1443</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="9" t="s">
-        <v>1456</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="9" t="s">
-        <v>1444</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="9" t="s">
-        <v>1445</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="50" t="s">
-        <v>1446</v>
-      </c>
-      <c r="B35" s="176"/>
-      <c r="C35" s="176"/>
-      <c r="D35" s="176"/>
-      <c r="E35" s="176"/>
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="9" t="s">
+        <v>1443</v>
+      </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="9" t="s">
-        <v>1447</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="9" t="s">
-        <v>1448</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="9" t="s">
-        <v>1449</v>
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="9" t="s">
+        <v>1445</v>
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="9" t="s">
-        <v>1457</v>
-      </c>
+      <c r="A40" s="50" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B40" s="176"/>
+      <c r="C40" s="176"/>
+      <c r="D40" s="176"/>
+      <c r="E40" s="176"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="9" t="s">
-        <v>1450</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="9" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="9" t="s">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="9" t="s">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="9" t="s">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="9" t="s">
         <v>1451</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="50" t="s">
-        <v>1441</v>
-      </c>
-      <c r="B44" s="176"/>
-      <c r="C44" s="176"/>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="9">
-        <f>MAX(PolicyLevers!H:H)</f>
-        <v>543</v>
-      </c>
-    </row>
+    <row r="49" spans="1:3" s="405" customFormat="1">
+      <c r="A49" s="403"/>
+      <c r="B49" s="404"/>
+      <c r="C49" s="404"/>
+    </row>
+    <row r="50" spans="1:3" s="405" customFormat="1"/>
   </sheetData>
+  <conditionalFormatting sqref="B18">
+    <cfRule type="containsText" dxfId="3" priority="3" stopIfTrue="1" operator="containsText" text="No duplicate ID numbers">
+      <formula>NOT(ISERROR(SEARCH("No duplicate ID numbers",B18)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="containsText" dxfId="1" priority="1" stopIfTrue="1" operator="containsText" text="No missing ID numbers">
+      <formula>NOT(ISERROR(SEARCH("No missing ID numbers",B19)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A10" r:id="rId1"/>
   </hyperlinks>
@@ -10915,8 +11017,8 @@
   <dimension ref="A1:T589"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A564" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N572" sqref="N572"/>
+      <pane ySplit="1" topLeftCell="A472" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H502" sqref="H502"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -15539,7 +15641,9 @@
       <c r="G77" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="H77" s="56"/>
+      <c r="H77" s="56">
+        <v>544</v>
+      </c>
       <c r="I77" s="10" t="s">
         <v>49</v>
       </c>
@@ -15602,7 +15706,9 @@
       <c r="G78" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="H78" s="56"/>
+      <c r="H78" s="56">
+        <v>545</v>
+      </c>
       <c r="I78" s="10" t="s">
         <v>49</v>
       </c>
@@ -15994,7 +16100,9 @@
       <c r="G86" s="77" t="s">
         <v>165</v>
       </c>
-      <c r="H86" s="56"/>
+      <c r="H86" s="56">
+        <v>546</v>
+      </c>
       <c r="I86" s="10" t="s">
         <v>49</v>
       </c>
@@ -16057,7 +16165,9 @@
       <c r="G87" s="77" t="s">
         <v>165</v>
       </c>
-      <c r="H87" s="56"/>
+      <c r="H87" s="56">
+        <v>547</v>
+      </c>
       <c r="I87" s="10" t="s">
         <v>49</v>
       </c>
@@ -17691,7 +17801,9 @@
       <c r="G112" s="55" t="s">
         <v>165</v>
       </c>
-      <c r="H112" s="56"/>
+      <c r="H112" s="56">
+        <v>548</v>
+      </c>
       <c r="I112" s="10" t="s">
         <v>49</v>
       </c>
@@ -35890,7 +36002,9 @@
       <c r="E426" s="55"/>
       <c r="F426" s="55"/>
       <c r="G426" s="55"/>
-      <c r="H426" s="56"/>
+      <c r="H426" s="56">
+        <v>549</v>
+      </c>
       <c r="I426" s="10" t="s">
         <v>49</v>
       </c>
@@ -37895,7 +38009,9 @@
         <v>953</v>
       </c>
       <c r="G465" s="55"/>
-      <c r="H465" s="56"/>
+      <c r="H465" s="56">
+        <v>550</v>
+      </c>
       <c r="I465" s="10" t="s">
         <v>49</v>
       </c>
@@ -39341,7 +39457,9 @@
         <v>957</v>
       </c>
       <c r="G496" s="57"/>
-      <c r="H496" s="56"/>
+      <c r="H496" s="56">
+        <v>551</v>
+      </c>
       <c r="I496" s="10" t="s">
         <v>49</v>
       </c>
@@ -39445,7 +39563,9 @@
         <v>498</v>
       </c>
       <c r="G498" s="57"/>
-      <c r="H498" s="56"/>
+      <c r="H498" s="56">
+        <v>552</v>
+      </c>
       <c r="I498" s="10" t="s">
         <v>49</v>
       </c>
@@ -39504,7 +39624,9 @@
         <v>952</v>
       </c>
       <c r="G499" s="57"/>
-      <c r="H499" s="56"/>
+      <c r="H499" s="56">
+        <v>553</v>
+      </c>
       <c r="I499" s="10" t="s">
         <v>49</v>
       </c>
@@ -39563,7 +39685,9 @@
         <v>959</v>
       </c>
       <c r="G500" s="57"/>
-      <c r="H500" s="56"/>
+      <c r="H500" s="56">
+        <v>554</v>
+      </c>
       <c r="I500" s="10" t="s">
         <v>49</v>
       </c>
@@ -39622,7 +39746,9 @@
         <v>953</v>
       </c>
       <c r="G501" s="57"/>
-      <c r="H501" s="56"/>
+      <c r="H501" s="56">
+        <v>555</v>
+      </c>
       <c r="I501" s="10" t="s">
         <v>49</v>
       </c>
@@ -43910,7 +44036,7 @@
       <c r="L571" s="196">
         <v>0</v>
       </c>
-      <c r="M571" s="399">
+      <c r="M571" s="390">
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="N571" s="207">
@@ -44135,232 +44261,232 @@
     <sortCondition ref="B119:B139"/>
   </sortState>
   <conditionalFormatting sqref="I66 I74 I22 I32 I42 I52">
-    <cfRule type="containsText" dxfId="51" priority="45" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="55" priority="45" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I75">
-    <cfRule type="containsText" dxfId="50" priority="44" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="54" priority="44" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I65">
-    <cfRule type="containsText" dxfId="49" priority="43" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="53" priority="43" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I67:I73">
-    <cfRule type="containsText" dxfId="48" priority="42" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="52" priority="42" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I89">
-    <cfRule type="containsText" dxfId="47" priority="41" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="51" priority="41" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I89)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I100">
-    <cfRule type="containsText" dxfId="46" priority="40" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="50" priority="40" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I100)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I519">
-    <cfRule type="containsText" dxfId="45" priority="39" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="49" priority="39" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I519)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I553">
-    <cfRule type="containsText" dxfId="44" priority="38" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="48" priority="38" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I553)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I60:I62">
-    <cfRule type="containsText" dxfId="43" priority="37" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="47" priority="37" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I50:I51">
-    <cfRule type="containsText" dxfId="42" priority="36" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="46" priority="36" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:I31">
-    <cfRule type="containsText" dxfId="41" priority="34" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="45" priority="34" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I21">
-    <cfRule type="containsText" dxfId="40" priority="33" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="44" priority="33" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I340">
-    <cfRule type="containsText" dxfId="39" priority="25" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="43" priority="25" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I350">
-    <cfRule type="containsText" dxfId="38" priority="24" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="42" priority="24" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I350)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I360">
-    <cfRule type="containsText" dxfId="37" priority="23" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="41" priority="23" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I360)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I370">
-    <cfRule type="containsText" dxfId="36" priority="22" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="40" priority="22" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I370)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I380">
-    <cfRule type="containsText" dxfId="35" priority="21" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="39" priority="21" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I380)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I390">
-    <cfRule type="containsText" dxfId="34" priority="20" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="38" priority="20" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I390)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I400">
-    <cfRule type="containsText" dxfId="33" priority="19" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="37" priority="19" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I400)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I337">
-    <cfRule type="containsText" dxfId="32" priority="18" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="36" priority="18" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I337)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I338:I339">
-    <cfRule type="containsText" dxfId="31" priority="17" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="35" priority="17" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I338)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I348:I349">
-    <cfRule type="containsText" dxfId="30" priority="16" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="34" priority="16" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I348)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I347">
-    <cfRule type="containsText" dxfId="29" priority="15" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="33" priority="15" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I347)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I358:I359">
-    <cfRule type="containsText" dxfId="28" priority="14" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="32" priority="14" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I358)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I357">
-    <cfRule type="containsText" dxfId="27" priority="13" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="31" priority="13" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I357)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I368">
-    <cfRule type="containsText" dxfId="26" priority="12" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="30" priority="12" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I368)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I367">
-    <cfRule type="containsText" dxfId="25" priority="11" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="29" priority="11" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I367)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I369">
-    <cfRule type="containsText" dxfId="24" priority="10" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="28" priority="10" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I369)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I388:I389">
-    <cfRule type="containsText" dxfId="23" priority="9" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="27" priority="9" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I388)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I387">
-    <cfRule type="containsText" dxfId="22" priority="8" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="26" priority="8" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I387)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I383">
-    <cfRule type="containsText" dxfId="21" priority="7" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="25" priority="7" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I383)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I385">
-    <cfRule type="containsText" dxfId="20" priority="6" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="24" priority="6" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I385)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I398:I399">
-    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I398)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I397">
-    <cfRule type="containsText" dxfId="18" priority="4" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="22" priority="4" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I397)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I536:I537">
-    <cfRule type="containsText" dxfId="17" priority="3" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="21" priority="3" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I536)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I570">
-    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="20" priority="2" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I570)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I76:I88 I520:I535 I554 I556:I569 I577:I1048576 I90:I99 I1:I9 I12:I19 I24 I33:I36 I43:I46 I53:I59 I38:I39 I48:I49 I63:I64 I341:I346 I351:I356 I361:I366 I381:I382 I391:I396 I371:I379 I384 I386 I538:I552 I571:I575 I113:I336 I401:I518">
-    <cfRule type="containsText" dxfId="15" priority="47" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="19" priority="47" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I555">
-    <cfRule type="containsText" dxfId="14" priority="46" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="18" priority="46" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I555)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40:I41">
-    <cfRule type="containsText" dxfId="13" priority="35" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="17" priority="35" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:I11">
-    <cfRule type="containsText" dxfId="12" priority="32" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="16" priority="32" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23">
-    <cfRule type="containsText" dxfId="11" priority="31" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="15" priority="31" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25:I29">
-    <cfRule type="containsText" dxfId="10" priority="30" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="14" priority="30" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="containsText" dxfId="9" priority="29" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="13" priority="29" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47">
-    <cfRule type="containsText" dxfId="8" priority="28" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="12" priority="28" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I101:I110">
-    <cfRule type="containsText" dxfId="7" priority="27" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="11" priority="27" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I101)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I111:I112">
-    <cfRule type="containsText" dxfId="6" priority="26" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="10" priority="26" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I111)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -44398,10 +44524,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="390" t="s">
+      <c r="A1" s="391" t="s">
         <v>1415</v>
       </c>
-      <c r="B1" s="390"/>
+      <c r="B1" s="391"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="166" t="s">
@@ -44687,10 +44813,10 @@
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="390" t="s">
+      <c r="A37" s="391" t="s">
         <v>1419</v>
       </c>
-      <c r="B37" s="390"/>
+      <c r="B37" s="391"/>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="166" t="s">
@@ -48564,26 +48690,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C74 C76:C80 C82:C136">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -54708,19 +54834,19 @@
       </c>
     </row>
     <row r="246" spans="1:11" s="95" customFormat="1" ht="15" customHeight="1">
-      <c r="A246" s="391" t="s">
+      <c r="A246" s="392" t="s">
         <v>1727</v>
       </c>
-      <c r="B246" s="392"/>
-      <c r="C246" s="392"/>
-      <c r="D246" s="392"/>
-      <c r="E246" s="392"/>
-      <c r="F246" s="392"/>
-      <c r="G246" s="392"/>
-      <c r="H246" s="392"/>
-      <c r="I246" s="392"/>
-      <c r="J246" s="392"/>
-      <c r="K246" s="393"/>
+      <c r="B246" s="393"/>
+      <c r="C246" s="393"/>
+      <c r="D246" s="393"/>
+      <c r="E246" s="393"/>
+      <c r="F246" s="393"/>
+      <c r="G246" s="393"/>
+      <c r="H246" s="393"/>
+      <c r="I246" s="393"/>
+      <c r="J246" s="393"/>
+      <c r="K246" s="394"/>
     </row>
     <row r="247" spans="1:11" s="95" customFormat="1"/>
     <row r="248" spans="1:11" s="95" customFormat="1" ht="28.5">
@@ -64399,22 +64525,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="394" t="s">
+      <c r="A1" s="398" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="394"/>
-      <c r="C1" s="394"/>
-      <c r="D1" s="394"/>
-      <c r="E1" s="394"/>
+      <c r="B1" s="398"/>
+      <c r="C1" s="398"/>
+      <c r="D1" s="398"/>
+      <c r="E1" s="398"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="398" t="s">
+      <c r="A2" s="399" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="398"/>
-      <c r="C2" s="398"/>
-      <c r="D2" s="398"/>
-      <c r="E2" s="398"/>
+      <c r="B2" s="399"/>
+      <c r="C2" s="399"/>
+      <c r="D2" s="399"/>
+      <c r="E2" s="399"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="9" t="s">
@@ -64430,13 +64556,13 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="398" t="s">
+      <c r="A21" s="399" t="s">
         <v>173</v>
       </c>
-      <c r="B21" s="398"/>
-      <c r="C21" s="398"/>
-      <c r="D21" s="398"/>
-      <c r="E21" s="398"/>
+      <c r="B21" s="399"/>
+      <c r="C21" s="399"/>
+      <c r="D21" s="399"/>
+      <c r="E21" s="399"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="9" t="s">
@@ -64452,13 +64578,13 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="398" t="s">
+      <c r="A40" s="399" t="s">
         <v>174</v>
       </c>
-      <c r="B40" s="398"/>
-      <c r="C40" s="398"/>
-      <c r="D40" s="398"/>
-      <c r="E40" s="398"/>
+      <c r="B40" s="399"/>
+      <c r="C40" s="399"/>
+      <c r="D40" s="399"/>
+      <c r="E40" s="399"/>
     </row>
     <row r="57" spans="1:5" ht="14.65" thickBot="1">
       <c r="A57" s="9" t="s">
@@ -64474,13 +64600,13 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="394" t="s">
+      <c r="A60" s="398" t="s">
         <v>176</v>
       </c>
-      <c r="B60" s="394"/>
-      <c r="C60" s="394"/>
-      <c r="D60" s="394"/>
-      <c r="E60" s="394"/>
+      <c r="B60" s="398"/>
+      <c r="C60" s="398"/>
+      <c r="D60" s="398"/>
+      <c r="E60" s="398"/>
     </row>
     <row r="85" spans="1:39" s="12" customFormat="1">
       <c r="A85" s="9" t="s">
@@ -64585,13 +64711,13 @@
       </c>
     </row>
     <row r="89" spans="1:39">
-      <c r="A89" s="394" t="s">
+      <c r="A89" s="398" t="s">
         <v>177</v>
       </c>
-      <c r="B89" s="394"/>
-      <c r="C89" s="394"/>
-      <c r="D89" s="394"/>
-      <c r="E89" s="394"/>
+      <c r="B89" s="398"/>
+      <c r="C89" s="398"/>
+      <c r="D89" s="398"/>
+      <c r="E89" s="398"/>
     </row>
     <row r="90" spans="1:39">
       <c r="A90" s="9">
@@ -64678,13 +64804,13 @@
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="394" t="s">
+      <c r="A98" s="398" t="s">
         <v>178</v>
       </c>
-      <c r="B98" s="394"/>
-      <c r="C98" s="394"/>
-      <c r="D98" s="394"/>
-      <c r="E98" s="394"/>
+      <c r="B98" s="398"/>
+      <c r="C98" s="398"/>
+      <c r="D98" s="398"/>
+      <c r="E98" s="398"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="17">
@@ -64768,13 +64894,13 @@
       <c r="A108" s="20"/>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="394" t="s">
+      <c r="A109" s="398" t="s">
         <v>180</v>
       </c>
-      <c r="B109" s="394"/>
-      <c r="C109" s="394"/>
-      <c r="D109" s="394"/>
-      <c r="E109" s="394"/>
+      <c r="B109" s="398"/>
+      <c r="C109" s="398"/>
+      <c r="D109" s="398"/>
+      <c r="E109" s="398"/>
     </row>
     <row r="110" spans="1:5" ht="14.65" thickBot="1"/>
     <row r="111" spans="1:5" ht="14.65" thickBot="1">
@@ -64787,13 +64913,13 @@
       </c>
     </row>
     <row r="113" spans="1:14">
-      <c r="A113" s="394" t="s">
+      <c r="A113" s="398" t="s">
         <v>179</v>
       </c>
-      <c r="B113" s="394"/>
-      <c r="C113" s="394"/>
-      <c r="D113" s="394"/>
-      <c r="E113" s="394"/>
+      <c r="B113" s="398"/>
+      <c r="C113" s="398"/>
+      <c r="D113" s="398"/>
+      <c r="E113" s="398"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="17">
@@ -64874,13 +65000,13 @@
       </c>
     </row>
     <row r="124" spans="1:14">
-      <c r="A124" s="394" t="s">
+      <c r="A124" s="398" t="s">
         <v>435</v>
       </c>
-      <c r="B124" s="394"/>
-      <c r="C124" s="394"/>
-      <c r="D124" s="394"/>
-      <c r="E124" s="394"/>
+      <c r="B124" s="398"/>
+      <c r="C124" s="398"/>
+      <c r="D124" s="398"/>
+      <c r="E124" s="398"/>
       <c r="L124" s="21"/>
     </row>
     <row r="125" spans="1:14">
@@ -64971,13 +65097,13 @@
       <c r="C133" s="15"/>
     </row>
     <row r="134" spans="1:14">
-      <c r="A134" s="394" t="s">
+      <c r="A134" s="398" t="s">
         <v>110</v>
       </c>
-      <c r="B134" s="394"/>
-      <c r="C134" s="394"/>
-      <c r="D134" s="394"/>
-      <c r="E134" s="394"/>
+      <c r="B134" s="398"/>
+      <c r="C134" s="398"/>
+      <c r="D134" s="398"/>
+      <c r="E134" s="398"/>
     </row>
     <row r="135" spans="1:14">
       <c r="A135" s="27" t="s">
@@ -65557,13 +65683,13 @@
       <c r="G163" s="28"/>
     </row>
     <row r="165" spans="1:7">
-      <c r="A165" s="394" t="s">
+      <c r="A165" s="398" t="s">
         <v>183</v>
       </c>
-      <c r="B165" s="394"/>
-      <c r="C165" s="394"/>
-      <c r="D165" s="394"/>
-      <c r="E165" s="394"/>
+      <c r="B165" s="398"/>
+      <c r="C165" s="398"/>
+      <c r="D165" s="398"/>
+      <c r="E165" s="398"/>
     </row>
     <row r="166" spans="1:7" ht="14.65" thickBot="1">
       <c r="A166" s="23" t="s">
@@ -65586,10 +65712,10 @@
       <c r="B168" s="46"/>
     </row>
     <row r="169" spans="1:7">
-      <c r="A169" s="394" t="s">
+      <c r="A169" s="398" t="s">
         <v>443</v>
       </c>
-      <c r="B169" s="394"/>
+      <c r="B169" s="398"/>
     </row>
     <row r="170" spans="1:7">
       <c r="A170" s="23" t="s">
@@ -65621,13 +65747,13 @@
       <c r="B173" s="46"/>
     </row>
     <row r="174" spans="1:7">
-      <c r="A174" s="394" t="s">
+      <c r="A174" s="398" t="s">
         <v>192</v>
       </c>
-      <c r="B174" s="394"/>
-      <c r="C174" s="394"/>
-      <c r="D174" s="394"/>
-      <c r="E174" s="394"/>
+      <c r="B174" s="398"/>
+      <c r="C174" s="398"/>
+      <c r="D174" s="398"/>
+      <c r="E174" s="398"/>
     </row>
     <row r="175" spans="1:7" ht="14.65" thickBot="1">
       <c r="A175" s="23" t="s">
@@ -65647,13 +65773,13 @@
       </c>
     </row>
     <row r="178" spans="1:5">
-      <c r="A178" s="394" t="s">
+      <c r="A178" s="398" t="s">
         <v>186</v>
       </c>
-      <c r="B178" s="394"/>
-      <c r="C178" s="394"/>
-      <c r="D178" s="394"/>
-      <c r="E178" s="394"/>
+      <c r="B178" s="398"/>
+      <c r="C178" s="398"/>
+      <c r="D178" s="398"/>
+      <c r="E178" s="398"/>
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="25" t="s">
@@ -65681,13 +65807,13 @@
       </c>
     </row>
     <row r="183" spans="1:5">
-      <c r="A183" s="394" t="s">
+      <c r="A183" s="398" t="s">
         <v>188</v>
       </c>
-      <c r="B183" s="394"/>
-      <c r="C183" s="394"/>
-      <c r="D183" s="394"/>
-      <c r="E183" s="394"/>
+      <c r="B183" s="398"/>
+      <c r="C183" s="398"/>
+      <c r="D183" s="398"/>
+      <c r="E183" s="398"/>
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="23" t="s">
@@ -65742,13 +65868,13 @@
       </c>
     </row>
     <row r="191" spans="1:5">
-      <c r="A191" s="394" t="s">
+      <c r="A191" s="398" t="s">
         <v>202</v>
       </c>
-      <c r="B191" s="394"/>
-      <c r="C191" s="394"/>
-      <c r="D191" s="394"/>
-      <c r="E191" s="394"/>
+      <c r="B191" s="398"/>
+      <c r="C191" s="398"/>
+      <c r="D191" s="398"/>
+      <c r="E191" s="398"/>
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="21" t="s">
@@ -65808,6 +65934,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -65822,12 +65954,6 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
WebAppData edit for building efficiency max slider bound
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -9626,9 +9626,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -9637,6 +9634,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -11022,8 +11022,8 @@
   <dimension ref="A1:T589"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I115" sqref="I115"/>
+      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M137" sqref="M137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -18987,7 +18987,7 @@
         <v>0</v>
       </c>
       <c r="M131" s="61">
-        <v>0</v>
+        <v>0.22</v>
       </c>
       <c r="N131" s="61">
         <v>0.01</v>
@@ -19055,7 +19055,7 @@
         <v>0</v>
       </c>
       <c r="M132" s="65">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="N132" s="63">
         <f t="shared" ref="N132:N148" si="54">N$131</f>
@@ -19131,7 +19131,7 @@
         <v>0</v>
       </c>
       <c r="M133" s="65">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="N133" s="63">
         <f t="shared" si="54"/>
@@ -19209,7 +19209,7 @@
         <v>0</v>
       </c>
       <c r="M134" s="65">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="N134" s="63">
         <f t="shared" si="54"/>
@@ -19287,7 +19287,7 @@
         <v>0</v>
       </c>
       <c r="M135" s="65">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="N135" s="63">
         <f t="shared" si="54"/>
@@ -19365,7 +19365,7 @@
         <v>0</v>
       </c>
       <c r="M136" s="65">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="N136" s="63">
         <f t="shared" si="54"/>
@@ -19444,7 +19444,7 @@
       </c>
       <c r="M137" s="63">
         <f>M131</f>
-        <v>0</v>
+        <v>0.22</v>
       </c>
       <c r="N137" s="63">
         <f t="shared" si="54"/>
@@ -19523,7 +19523,7 @@
       </c>
       <c r="M138" s="63">
         <f t="shared" ref="M138:M142" si="58">M132</f>
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="N138" s="63">
         <f t="shared" si="54"/>
@@ -19602,7 +19602,7 @@
       </c>
       <c r="M139" s="63">
         <f t="shared" si="58"/>
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="N139" s="63">
         <f t="shared" si="54"/>
@@ -19681,7 +19681,7 @@
       </c>
       <c r="M140" s="63">
         <f t="shared" si="58"/>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="N140" s="63">
         <f t="shared" si="54"/>
@@ -19760,7 +19760,7 @@
       </c>
       <c r="M141" s="63">
         <f t="shared" si="58"/>
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="N141" s="63">
         <f t="shared" si="54"/>
@@ -19839,7 +19839,7 @@
       </c>
       <c r="M142" s="63">
         <f t="shared" si="58"/>
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="N142" s="63">
         <f t="shared" si="54"/>
@@ -19918,7 +19918,7 @@
       </c>
       <c r="M143" s="63">
         <f>M137</f>
-        <v>0</v>
+        <v>0.22</v>
       </c>
       <c r="N143" s="63">
         <f t="shared" si="54"/>
@@ -64546,13 +64546,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="398" t="s">
+      <c r="A1" s="401" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="398"/>
-      <c r="C1" s="398"/>
-      <c r="D1" s="398"/>
-      <c r="E1" s="398"/>
+      <c r="B1" s="401"/>
+      <c r="C1" s="401"/>
+      <c r="D1" s="401"/>
+      <c r="E1" s="401"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="402" t="s">
@@ -64621,13 +64621,13 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="398" t="s">
+      <c r="A60" s="401" t="s">
         <v>176</v>
       </c>
-      <c r="B60" s="398"/>
-      <c r="C60" s="398"/>
-      <c r="D60" s="398"/>
-      <c r="E60" s="398"/>
+      <c r="B60" s="401"/>
+      <c r="C60" s="401"/>
+      <c r="D60" s="401"/>
+      <c r="E60" s="401"/>
     </row>
     <row r="85" spans="1:39" s="12" customFormat="1">
       <c r="A85" s="9" t="s">
@@ -64732,13 +64732,13 @@
       </c>
     </row>
     <row r="89" spans="1:39">
-      <c r="A89" s="398" t="s">
+      <c r="A89" s="401" t="s">
         <v>177</v>
       </c>
-      <c r="B89" s="398"/>
-      <c r="C89" s="398"/>
-      <c r="D89" s="398"/>
-      <c r="E89" s="398"/>
+      <c r="B89" s="401"/>
+      <c r="C89" s="401"/>
+      <c r="D89" s="401"/>
+      <c r="E89" s="401"/>
     </row>
     <row r="90" spans="1:39">
       <c r="A90" s="9">
@@ -64825,13 +64825,13 @@
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="398" t="s">
+      <c r="A98" s="401" t="s">
         <v>178</v>
       </c>
-      <c r="B98" s="398"/>
-      <c r="C98" s="398"/>
-      <c r="D98" s="398"/>
-      <c r="E98" s="398"/>
+      <c r="B98" s="401"/>
+      <c r="C98" s="401"/>
+      <c r="D98" s="401"/>
+      <c r="E98" s="401"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="17">
@@ -64915,13 +64915,13 @@
       <c r="A108" s="20"/>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="398" t="s">
+      <c r="A109" s="401" t="s">
         <v>180</v>
       </c>
-      <c r="B109" s="398"/>
-      <c r="C109" s="398"/>
-      <c r="D109" s="398"/>
-      <c r="E109" s="398"/>
+      <c r="B109" s="401"/>
+      <c r="C109" s="401"/>
+      <c r="D109" s="401"/>
+      <c r="E109" s="401"/>
     </row>
     <row r="110" spans="1:5" ht="14.65" thickBot="1"/>
     <row r="111" spans="1:5" ht="14.65" thickBot="1">
@@ -64934,13 +64934,13 @@
       </c>
     </row>
     <row r="113" spans="1:14">
-      <c r="A113" s="398" t="s">
+      <c r="A113" s="401" t="s">
         <v>179</v>
       </c>
-      <c r="B113" s="398"/>
-      <c r="C113" s="398"/>
-      <c r="D113" s="398"/>
-      <c r="E113" s="398"/>
+      <c r="B113" s="401"/>
+      <c r="C113" s="401"/>
+      <c r="D113" s="401"/>
+      <c r="E113" s="401"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="17">
@@ -65021,13 +65021,13 @@
       </c>
     </row>
     <row r="124" spans="1:14">
-      <c r="A124" s="398" t="s">
+      <c r="A124" s="401" t="s">
         <v>435</v>
       </c>
-      <c r="B124" s="398"/>
-      <c r="C124" s="398"/>
-      <c r="D124" s="398"/>
-      <c r="E124" s="398"/>
+      <c r="B124" s="401"/>
+      <c r="C124" s="401"/>
+      <c r="D124" s="401"/>
+      <c r="E124" s="401"/>
       <c r="L124" s="21"/>
     </row>
     <row r="125" spans="1:14">
@@ -65118,13 +65118,13 @@
       <c r="C133" s="15"/>
     </row>
     <row r="134" spans="1:14">
-      <c r="A134" s="398" t="s">
+      <c r="A134" s="401" t="s">
         <v>110</v>
       </c>
-      <c r="B134" s="398"/>
-      <c r="C134" s="398"/>
-      <c r="D134" s="398"/>
-      <c r="E134" s="398"/>
+      <c r="B134" s="401"/>
+      <c r="C134" s="401"/>
+      <c r="D134" s="401"/>
+      <c r="E134" s="401"/>
     </row>
     <row r="135" spans="1:14">
       <c r="A135" s="27" t="s">
@@ -65139,25 +65139,25 @@
     </row>
     <row r="136" spans="1:14">
       <c r="A136" s="29"/>
-      <c r="B136" s="399" t="s">
+      <c r="B136" s="398" t="s">
         <v>452</v>
       </c>
-      <c r="C136" s="400"/>
-      <c r="D136" s="400"/>
-      <c r="E136" s="401"/>
+      <c r="C136" s="399"/>
+      <c r="D136" s="399"/>
+      <c r="E136" s="400"/>
       <c r="F136" s="28"/>
       <c r="G136" s="28"/>
     </row>
     <row r="137" spans="1:14">
       <c r="A137" s="30"/>
-      <c r="B137" s="399" t="s">
+      <c r="B137" s="398" t="s">
         <v>453</v>
       </c>
-      <c r="C137" s="401"/>
-      <c r="D137" s="399" t="s">
+      <c r="C137" s="400"/>
+      <c r="D137" s="398" t="s">
         <v>454</v>
       </c>
-      <c r="E137" s="401"/>
+      <c r="E137" s="400"/>
       <c r="F137" s="28"/>
       <c r="G137" s="28"/>
     </row>
@@ -65704,13 +65704,13 @@
       <c r="G163" s="28"/>
     </row>
     <row r="165" spans="1:7">
-      <c r="A165" s="398" t="s">
+      <c r="A165" s="401" t="s">
         <v>183</v>
       </c>
-      <c r="B165" s="398"/>
-      <c r="C165" s="398"/>
-      <c r="D165" s="398"/>
-      <c r="E165" s="398"/>
+      <c r="B165" s="401"/>
+      <c r="C165" s="401"/>
+      <c r="D165" s="401"/>
+      <c r="E165" s="401"/>
     </row>
     <row r="166" spans="1:7" ht="14.65" thickBot="1">
       <c r="A166" s="23" t="s">
@@ -65733,10 +65733,10 @@
       <c r="B168" s="46"/>
     </row>
     <row r="169" spans="1:7">
-      <c r="A169" s="398" t="s">
+      <c r="A169" s="401" t="s">
         <v>443</v>
       </c>
-      <c r="B169" s="398"/>
+      <c r="B169" s="401"/>
     </row>
     <row r="170" spans="1:7">
       <c r="A170" s="23" t="s">
@@ -65768,13 +65768,13 @@
       <c r="B173" s="46"/>
     </row>
     <row r="174" spans="1:7">
-      <c r="A174" s="398" t="s">
+      <c r="A174" s="401" t="s">
         <v>192</v>
       </c>
-      <c r="B174" s="398"/>
-      <c r="C174" s="398"/>
-      <c r="D174" s="398"/>
-      <c r="E174" s="398"/>
+      <c r="B174" s="401"/>
+      <c r="C174" s="401"/>
+      <c r="D174" s="401"/>
+      <c r="E174" s="401"/>
     </row>
     <row r="175" spans="1:7" ht="14.65" thickBot="1">
       <c r="A175" s="23" t="s">
@@ -65794,13 +65794,13 @@
       </c>
     </row>
     <row r="178" spans="1:5">
-      <c r="A178" s="398" t="s">
+      <c r="A178" s="401" t="s">
         <v>186</v>
       </c>
-      <c r="B178" s="398"/>
-      <c r="C178" s="398"/>
-      <c r="D178" s="398"/>
-      <c r="E178" s="398"/>
+      <c r="B178" s="401"/>
+      <c r="C178" s="401"/>
+      <c r="D178" s="401"/>
+      <c r="E178" s="401"/>
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="25" t="s">
@@ -65828,13 +65828,13 @@
       </c>
     </row>
     <row r="183" spans="1:5">
-      <c r="A183" s="398" t="s">
+      <c r="A183" s="401" t="s">
         <v>188</v>
       </c>
-      <c r="B183" s="398"/>
-      <c r="C183" s="398"/>
-      <c r="D183" s="398"/>
-      <c r="E183" s="398"/>
+      <c r="B183" s="401"/>
+      <c r="C183" s="401"/>
+      <c r="D183" s="401"/>
+      <c r="E183" s="401"/>
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="23" t="s">
@@ -65889,13 +65889,13 @@
       </c>
     </row>
     <row r="191" spans="1:5">
-      <c r="A191" s="398" t="s">
+      <c r="A191" s="401" t="s">
         <v>202</v>
       </c>
-      <c r="B191" s="398"/>
-      <c r="C191" s="398"/>
-      <c r="D191" s="398"/>
-      <c r="E191" s="398"/>
+      <c r="B191" s="401"/>
+      <c r="C191" s="401"/>
+      <c r="D191" s="401"/>
+      <c r="E191" s="401"/>
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="21" t="s">
@@ -65955,6 +65955,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -65969,12 +65975,6 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Copy edit to WebAppData
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -25,16 +25,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PolicyLevers!$A$1:$T$571</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -5704,9 +5694,6 @@
     <t>**Description:** This policy increases the tax rate for LPG.  It is expressed as a percentage of the BAU Scenario price, which includes sales and excise taxes. // **Guidance for setting values:**  In 2018, the national and state-level Goods and Services Tax (GST) rates on domestic LPG were 2.5% each, adding up to a national average tax rate of 5%.</t>
   </si>
   <si>
-    <t>**Description:** This control setting adjusts the GDP impact of the recession caused by SARS-CoV-2 (COVID-19).  It is set in terms of the GDP growth rate for 2020, relative to 2019 (with negative values indicating GDP shrinkage).  Recession impacts can extend beyond 2020, and can be adjusted using the Implementation Schedule feature for this control setting.  // **Guidance for setting values:** As of April 2020, projections for GDP impacts in India vary across several studies. Estimates by six national and global agencies range between a GDP shrinkage of 0.5% on the optimistic end to a high of 5.4% (relative to counter-factual growth projections of 5%-6%). On average, the projected shrinkage is 3.2%, which is the default setting.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -7497,6 +7484,9 @@
   </si>
   <si>
     <t>Scenario_Post2030Policies.cin</t>
+  </si>
+  <si>
+    <t>**Description:** This control setting adjusts the GDP impact of the recession caused by SARS-CoV-2 (COVID-19).  It is set in terms of the GDP growth rate for 2020, relative to 2019 (with negative values indicating GDP shrinkage).  Recession impacts can extend beyond 2020, and can be adjusted using the Implementation Schedule feature for this control setting.  // **Guidance for setting values:** As of 27 May 2020, projections for GDP impacts in India vary across several studies. Estimates by nine national and global agencies range between a GDP reduction of 2.3% on the optimistic end to a high of 11% (relative to an average counter-factual growth projection of 5.8%). On average, the projected reduction is 5.9%, resulting in a new GDP growth rate of -0.1%. This is the default setting.</t>
   </si>
 </sst>
 </file>
@@ -8564,7 +8554,7 @@
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="403">
+  <cellXfs count="404">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -9610,6 +9600,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="30" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -9622,9 +9615,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -9634,10 +9624,13 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="30" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -10841,7 +10834,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="50" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="B16" s="176"/>
     </row>
@@ -10856,7 +10849,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="391" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="B18" s="118" t="str">
         <f t="array" ref="B18">IF(MIN(IF(COUNTIF(PolicyLevers!$H$2:$H$1500,PolicyLevers!$H$2:$H$1500)&gt;1,PolicyLevers!$H$2:$H$1500, ""))=0,"No duplicate ID numbers",MIN(IF(COUNTIF(PolicyLevers!$H$2:$H$1500,PolicyLevers!$H$2:$H$1500)&gt;1,PolicyLevers!$H$2:$H$1500, "")))</f>
@@ -10865,7 +10858,7 @@
     </row>
     <row r="19" spans="1:6" ht="28.5">
       <c r="A19" s="392" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="B19" s="118" t="str">
         <f>IF(MIN(IF((NOT(ISNUMBER(PolicyLevers!$H$2:$H$1500)))*(PolicyLevers!$I$2:$I$1500="Yes"),ROW(PolicyLevers!$H$2:$H$1500)))=0,"No missing ID numbers",MIN(IF((NOT(ISNUMBER(PolicyLevers!$H$2:$H$1500)))*(PolicyLevers!$I$2:$I$1500="Yes"),ROW(PolicyLevers!$H$2:$H$1500))))</f>
@@ -11022,7 +11015,7 @@
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A564" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N571" sqref="N571"/>
+      <selection pane="bottomLeft" activeCell="P571" sqref="P571"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -11165,7 +11158,7 @@
         <v>823</v>
       </c>
       <c r="S2" s="71" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="T2" s="99"/>
     </row>
@@ -11236,7 +11229,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S3" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="4" spans="1:20" s="3" customFormat="1" ht="57">
@@ -11306,7 +11299,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S4" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="3" customFormat="1" ht="57">
@@ -11376,7 +11369,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S5" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="6" spans="1:20" s="3" customFormat="1" ht="57">
@@ -11446,7 +11439,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S6" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="7" spans="1:20" s="3" customFormat="1" ht="28.5">
@@ -11576,7 +11569,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S8" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="9" spans="1:20" s="3" customFormat="1" ht="57">
@@ -11646,7 +11639,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S9" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="10" spans="1:20" s="3" customFormat="1" ht="28.5">
@@ -11800,7 +11793,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S12" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="13" spans="1:20" s="3" customFormat="1" ht="57">
@@ -11870,7 +11863,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S13" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="14" spans="1:20" s="3" customFormat="1" ht="57">
@@ -11940,7 +11933,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S14" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="15" spans="1:20" s="3" customFormat="1" ht="57">
@@ -12010,7 +12003,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S15" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="16" spans="1:20" s="3" customFormat="1" ht="57">
@@ -12080,7 +12073,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S16" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="17" spans="1:19" s="3" customFormat="1" ht="28.5">
@@ -12210,7 +12203,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S18" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="19" spans="1:19" s="3" customFormat="1" ht="57">
@@ -12280,7 +12273,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S19" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="20" spans="1:19" s="3" customFormat="1" ht="28.5">
@@ -12434,7 +12427,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S22" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="23" spans="1:19" s="3" customFormat="1" ht="28.5">
@@ -12546,7 +12539,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S24" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="25" spans="1:19" s="3" customFormat="1" ht="28.5">
@@ -12910,7 +12903,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S32" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="33" spans="1:19" s="3" customFormat="1" ht="57">
@@ -12980,7 +12973,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S33" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="34" spans="1:19" s="3" customFormat="1" ht="57">
@@ -13050,7 +13043,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S34" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="35" spans="1:19" s="3" customFormat="1" ht="57">
@@ -13120,7 +13113,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S35" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="36" spans="1:19" s="3" customFormat="1" ht="57">
@@ -13190,7 +13183,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S36" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="37" spans="1:19" s="3" customFormat="1" ht="28.5">
@@ -13302,7 +13295,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S38" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="39" spans="1:19" s="3" customFormat="1" ht="57">
@@ -13372,7 +13365,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S39" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="40" spans="1:19" s="3" customFormat="1" ht="28.5">
@@ -13526,7 +13519,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S42" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="43" spans="1:19" s="3" customFormat="1" ht="57">
@@ -13596,7 +13589,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S43" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="44" spans="1:19" s="3" customFormat="1" ht="57">
@@ -13666,7 +13659,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S44" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="45" spans="1:19" s="3" customFormat="1" ht="57">
@@ -13736,7 +13729,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S45" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="46" spans="1:19" s="3" customFormat="1" ht="57">
@@ -13806,7 +13799,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S46" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="47" spans="1:19" s="3" customFormat="1" ht="28.5">
@@ -13918,7 +13911,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S48" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="49" spans="1:20" s="3" customFormat="1" ht="57">
@@ -13988,7 +13981,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S49" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="50" spans="1:20" s="3" customFormat="1" ht="28.5">
@@ -14142,7 +14135,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S52" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="53" spans="1:20" s="3" customFormat="1" ht="57">
@@ -14212,7 +14205,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S53" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="54" spans="1:20" s="3" customFormat="1" ht="57">
@@ -14282,7 +14275,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S54" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="55" spans="1:20" s="3" customFormat="1" ht="57">
@@ -14352,7 +14345,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S55" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="56" spans="1:20" s="3" customFormat="1" ht="57">
@@ -14422,7 +14415,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S56" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="57" spans="1:20" s="3" customFormat="1" ht="28.5">
@@ -14552,7 +14545,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S58" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="59" spans="1:20" s="3" customFormat="1" ht="57">
@@ -14622,7 +14615,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
       <c r="S59" s="108" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="60" spans="1:20" s="3" customFormat="1" ht="28.5">
@@ -14750,7 +14743,7 @@
         <v>1237</v>
       </c>
       <c r="S62" s="71" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="T62" s="99"/>
     </row>
@@ -14800,7 +14793,7 @@
         <v>1238</v>
       </c>
       <c r="S63" s="75" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="T63" s="10"/>
     </row>
@@ -14860,7 +14853,7 @@
         <v>524</v>
       </c>
       <c r="S64" s="185" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="T64" s="10"/>
     </row>
@@ -15509,7 +15502,7 @@
         <v>ev-mandate.html</v>
       </c>
       <c r="S74" s="187" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="T74" s="10"/>
     </row>
@@ -15616,7 +15609,7 @@
         <v>517</v>
       </c>
       <c r="S76" s="75" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="T76" s="10"/>
     </row>
@@ -15681,7 +15674,7 @@
       <c r="Q77" s="79"/>
       <c r="R77" s="157"/>
       <c r="S77" s="75" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="T77" s="96"/>
     </row>
@@ -15746,7 +15739,7 @@
       <c r="Q78" s="79"/>
       <c r="R78" s="157"/>
       <c r="S78" s="75" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="T78" s="96"/>
     </row>
@@ -16140,7 +16133,7 @@
       <c r="Q86" s="79"/>
       <c r="R86" s="157"/>
       <c r="S86" s="75" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="T86" s="96"/>
     </row>
@@ -16205,7 +16198,7 @@
       <c r="Q87" s="79"/>
       <c r="R87" s="157"/>
       <c r="S87" s="75" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="T87" s="96"/>
     </row>
@@ -16319,7 +16312,7 @@
         <v>211</v>
       </c>
       <c r="S89" s="188" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="T89" s="182" t="s">
         <v>412</v>
@@ -16392,7 +16385,7 @@
         <v>fuel-economy-standard.html</v>
       </c>
       <c r="S90" s="188" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="T90" s="182" t="s">
         <v>412</v>
@@ -16464,7 +16457,7 @@
         <v>fuel-economy-standard.html</v>
       </c>
       <c r="S91" s="188" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="T91" s="182" t="s">
         <v>423</v>
@@ -16537,7 +16530,7 @@
         <v>fuel-economy-standard.html</v>
       </c>
       <c r="S92" s="188" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="T92" s="182" t="s">
         <v>423</v>
@@ -16609,7 +16602,7 @@
         <v>fuel-economy-standard.html</v>
       </c>
       <c r="S93" s="182" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="T93" s="182" t="s">
         <v>190</v>
@@ -16682,7 +16675,7 @@
         <v>fuel-economy-standard.html</v>
       </c>
       <c r="S94" s="182" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="T94" s="106" t="str">
         <f>T$93</f>
@@ -16755,7 +16748,7 @@
         <v>fuel-economy-standard.html</v>
       </c>
       <c r="S95" s="182" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="T95" s="55" t="s">
         <v>191</v>
@@ -16817,7 +16810,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P96" s="177" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="Q96" s="76" t="str">
         <f t="shared" si="23"/>
@@ -16828,7 +16821,7 @@
         <v>fuel-economy-standard.html</v>
       </c>
       <c r="S96" s="182" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="T96" s="106" t="str">
         <f>T$95</f>
@@ -16901,7 +16894,7 @@
         <v>fuel-economy-standard.html</v>
       </c>
       <c r="S97" s="182" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="T97" s="55" t="s">
         <v>190</v>
@@ -16974,7 +16967,7 @@
         <v>fuel-economy-standard.html</v>
       </c>
       <c r="S98" s="182" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="T98" s="106" t="str">
         <f>T$97</f>
@@ -17047,7 +17040,7 @@
         <v>fuel-economy-standard.html</v>
       </c>
       <c r="S99" s="182" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="T99" s="55" t="s">
         <v>441</v>
@@ -17156,7 +17149,7 @@
         <v>1239</v>
       </c>
       <c r="S101" s="189" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="T101" s="10"/>
     </row>
@@ -17224,7 +17217,7 @@
         <v>hydrogen-vehicle-mandate.html</v>
       </c>
       <c r="S102" s="55" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="T102" s="55"/>
     </row>
@@ -17292,7 +17285,7 @@
         <v>hydrogen-vehicle-mandate.html</v>
       </c>
       <c r="S103" s="55" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="T103" s="55"/>
     </row>
@@ -17360,7 +17353,7 @@
         <v>hydrogen-vehicle-mandate.html</v>
       </c>
       <c r="S104" s="55" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="T104" s="55"/>
     </row>
@@ -17834,7 +17827,7 @@
       <c r="Q112" s="57"/>
       <c r="R112" s="159"/>
       <c r="S112" s="55" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="T112" s="55"/>
     </row>
@@ -17886,7 +17879,7 @@
         <v>530</v>
       </c>
       <c r="S113" s="10" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="T113" s="10"/>
     </row>
@@ -18070,7 +18063,7 @@
         <v>215</v>
       </c>
       <c r="S116" s="10" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="T116" s="55"/>
     </row>
@@ -18117,7 +18110,7 @@
       <c r="Q117" s="60"/>
       <c r="R117" s="160"/>
       <c r="S117" s="57" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="T117" s="60"/>
     </row>
@@ -18164,7 +18157,7 @@
       <c r="Q118" s="60"/>
       <c r="R118" s="160"/>
       <c r="S118" s="57" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="T118" s="60"/>
     </row>
@@ -18235,7 +18228,7 @@
         <v>building-component-electrification.html</v>
       </c>
       <c r="S119" s="57" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="T119" s="60"/>
     </row>
@@ -18306,7 +18299,7 @@
         <v>building-component-electrification.html</v>
       </c>
       <c r="S120" s="57" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="T120" s="60"/>
     </row>
@@ -18377,7 +18370,7 @@
         <v>building-component-electrification.html</v>
       </c>
       <c r="S121" s="57" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="T121" s="60"/>
     </row>
@@ -18424,7 +18417,7 @@
       <c r="Q122" s="60"/>
       <c r="R122" s="160"/>
       <c r="S122" s="57" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="T122" s="60"/>
     </row>
@@ -18483,7 +18476,7 @@
       <c r="Q123" s="60"/>
       <c r="R123" s="160"/>
       <c r="S123" s="57" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="T123" s="60"/>
     </row>
@@ -18554,7 +18547,7 @@
         <v>building-component-electrification.html</v>
       </c>
       <c r="S124" s="57" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="T124" s="60"/>
     </row>
@@ -18625,7 +18618,7 @@
         <v>building-component-electrification.html</v>
       </c>
       <c r="S125" s="57" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="T125" s="60"/>
     </row>
@@ -18696,7 +18689,7 @@
         <v>building-component-electrification.html</v>
       </c>
       <c r="S126" s="57" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="T126" s="60"/>
     </row>
@@ -18743,7 +18736,7 @@
       <c r="Q127" s="60"/>
       <c r="R127" s="160"/>
       <c r="S127" s="57" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="T127" s="60"/>
     </row>
@@ -18802,7 +18795,7 @@
       <c r="Q128" s="60"/>
       <c r="R128" s="160"/>
       <c r="S128" s="57" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="T128" s="60"/>
     </row>
@@ -18873,7 +18866,7 @@
         <v>building-component-electrification.html</v>
       </c>
       <c r="S129" s="57" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="T129" s="60"/>
     </row>
@@ -18944,7 +18937,7 @@
         <v>building-component-electrification.html</v>
       </c>
       <c r="S130" s="57" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="T130" s="60"/>
     </row>
@@ -19004,7 +18997,7 @@
         <v>217</v>
       </c>
       <c r="S131" s="185" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="T131" s="55" t="s">
         <v>479</v>
@@ -19076,7 +19069,7 @@
         <v>building-energy-efficiency-standards.html</v>
       </c>
       <c r="S132" s="190" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="T132" s="57" t="str">
         <f>T131</f>
@@ -20013,10 +20006,10 @@
         <v>building-energy-efficiency-standards.html</v>
       </c>
       <c r="S144" s="57" t="s">
+        <v>1644</v>
+      </c>
+      <c r="T144" s="57" t="s">
         <v>1645</v>
-      </c>
-      <c r="T144" s="57" t="s">
-        <v>1646</v>
       </c>
     </row>
     <row r="145" spans="1:20" s="5" customFormat="1" ht="85.5">
@@ -20085,10 +20078,10 @@
         <v>building-energy-efficiency-standards.html</v>
       </c>
       <c r="S145" s="57" t="s">
+        <v>1644</v>
+      </c>
+      <c r="T145" s="57" t="s">
         <v>1645</v>
-      </c>
-      <c r="T145" s="57" t="s">
-        <v>1646</v>
       </c>
     </row>
     <row r="146" spans="1:20" s="5" customFormat="1" ht="85.5">
@@ -20157,10 +20150,10 @@
         <v>building-energy-efficiency-standards.html</v>
       </c>
       <c r="S146" s="57" t="s">
+        <v>1644</v>
+      </c>
+      <c r="T146" s="57" t="s">
         <v>1645</v>
-      </c>
-      <c r="T146" s="57" t="s">
-        <v>1646</v>
       </c>
     </row>
     <row r="147" spans="1:20" s="5" customFormat="1" ht="85.5">
@@ -20229,10 +20222,10 @@
         <v>building-energy-efficiency-standards.html</v>
       </c>
       <c r="S147" s="57" t="s">
+        <v>1644</v>
+      </c>
+      <c r="T147" s="57" t="s">
         <v>1645</v>
-      </c>
-      <c r="T147" s="57" t="s">
-        <v>1646</v>
       </c>
     </row>
     <row r="148" spans="1:20" s="5" customFormat="1" ht="85.5">
@@ -20301,10 +20294,10 @@
         <v>building-energy-efficiency-standards.html</v>
       </c>
       <c r="S148" s="57" t="s">
+        <v>1644</v>
+      </c>
+      <c r="T148" s="57" t="s">
         <v>1645</v>
-      </c>
-      <c r="T148" s="57" t="s">
-        <v>1646</v>
       </c>
     </row>
     <row r="149" spans="1:20" s="5" customFormat="1" ht="57">
@@ -20407,7 +20400,7 @@
         <v>289</v>
       </c>
       <c r="S150" s="10" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="T150" s="10"/>
     </row>
@@ -20459,7 +20452,7 @@
         <v>292</v>
       </c>
       <c r="S151" s="10" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="T151" s="57"/>
     </row>
@@ -20511,7 +20504,7 @@
         <v>221</v>
       </c>
       <c r="S152" s="10" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="T152" s="57"/>
     </row>
@@ -20567,7 +20560,7 @@
         <v>223</v>
       </c>
       <c r="S153" s="10" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="T153" s="10"/>
     </row>
@@ -21842,7 +21835,7 @@
         <v>39</v>
       </c>
       <c r="P178" s="180" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="Q178" s="55" t="s">
         <v>926</v>
@@ -21851,7 +21844,7 @@
         <v>927</v>
       </c>
       <c r="S178" s="10" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="T178" s="55"/>
     </row>
@@ -21903,7 +21896,7 @@
         <v>303</v>
       </c>
       <c r="S179" s="10" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="T179" s="10"/>
     </row>
@@ -21959,7 +21952,7 @@
         <v>303</v>
       </c>
       <c r="S180" s="10" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="T180" s="10"/>
     </row>
@@ -23057,7 +23050,7 @@
         <v>227</v>
       </c>
       <c r="S197" s="55" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="T197" s="55"/>
     </row>
@@ -23113,7 +23106,7 @@
         <v>229</v>
       </c>
       <c r="S198" s="55" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="T198" s="55"/>
     </row>
@@ -23223,7 +23216,7 @@
         <v>229</v>
       </c>
       <c r="S200" s="55" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="T200" s="55"/>
     </row>
@@ -23844,7 +23837,7 @@
         <v>231</v>
       </c>
       <c r="S214" s="55" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="T214" s="55"/>
     </row>
@@ -23896,7 +23889,7 @@
         <v>233</v>
       </c>
       <c r="S215" s="55" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="T215" s="55"/>
     </row>
@@ -26866,7 +26859,7 @@
         <v>276</v>
       </c>
       <c r="S282" s="10" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="T282" s="10"/>
     </row>
@@ -27158,7 +27151,7 @@
       </c>
       <c r="R287" s="158"/>
       <c r="S287" s="150" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="T287" s="10"/>
     </row>
@@ -27222,7 +27215,7 @@
       </c>
       <c r="R288" s="158"/>
       <c r="S288" s="150" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="T288" s="10"/>
     </row>
@@ -27286,7 +27279,7 @@
       </c>
       <c r="R289" s="158"/>
       <c r="S289" s="150" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="T289" s="10"/>
     </row>
@@ -27350,7 +27343,7 @@
       </c>
       <c r="R290" s="158"/>
       <c r="S290" s="150" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="T290" s="10"/>
     </row>
@@ -27472,7 +27465,7 @@
       </c>
       <c r="R292" s="158"/>
       <c r="S292" s="150" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="T292" s="10"/>
     </row>
@@ -27793,7 +27786,7 @@
         <v>236</v>
       </c>
       <c r="S298" s="188" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="T298" s="55"/>
     </row>
@@ -28395,7 +28388,7 @@
         <v>238</v>
       </c>
       <c r="S309" s="182" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="T309" s="55"/>
     </row>
@@ -28447,7 +28440,7 @@
         <v>240</v>
       </c>
       <c r="S310" s="55" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="T310" s="57"/>
     </row>
@@ -28499,7 +28492,7 @@
         <v>242</v>
       </c>
       <c r="S311" s="55" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="T311" s="57"/>
     </row>
@@ -28555,7 +28548,7 @@
         <v>244</v>
       </c>
       <c r="S312" s="191" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="T312" s="10" t="s">
         <v>585</v>
@@ -28951,7 +28944,7 @@
         <v>244</v>
       </c>
       <c r="S318" s="57" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="T318" s="57" t="str">
         <f t="shared" si="105"/>
@@ -29072,7 +29065,7 @@
         <v>246</v>
       </c>
       <c r="S320" s="55" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="T320" s="57"/>
     </row>
@@ -34539,7 +34532,7 @@
         <v>589</v>
       </c>
       <c r="S401" s="10" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="T401" s="10"/>
     </row>
@@ -34591,7 +34584,7 @@
         <v>589</v>
       </c>
       <c r="S402" s="10" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="T402" s="10"/>
     </row>
@@ -34643,7 +34636,7 @@
         <v>589</v>
       </c>
       <c r="S403" s="10" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="T403" s="10"/>
     </row>
@@ -34695,7 +34688,7 @@
         <v>589</v>
       </c>
       <c r="S404" s="10" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="T404" s="10"/>
     </row>
@@ -35058,7 +35051,7 @@
         <v>249</v>
       </c>
       <c r="S410" s="10" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="T410" s="55"/>
     </row>
@@ -35441,7 +35434,7 @@
         <v>1242</v>
       </c>
       <c r="S416" s="55" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="T416" s="55"/>
     </row>
@@ -35986,7 +35979,7 @@
         <v>253</v>
       </c>
       <c r="S425" s="55" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="T425" s="182" t="s">
         <v>203</v>
@@ -36040,7 +36033,7 @@
         <v>348</v>
       </c>
       <c r="S426" s="55" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="T426" s="55"/>
     </row>
@@ -36090,7 +36083,7 @@
         <v>1248</v>
       </c>
       <c r="S427" s="55" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="T427" s="55"/>
     </row>
@@ -36142,7 +36135,7 @@
         <v>255</v>
       </c>
       <c r="S428" s="55" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="T428" s="55"/>
     </row>
@@ -36194,7 +36187,7 @@
         <v>257</v>
       </c>
       <c r="S429" s="55" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="T429" s="55"/>
     </row>
@@ -36246,7 +36239,7 @@
         <v>259</v>
       </c>
       <c r="S430" s="55" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="T430" s="55"/>
     </row>
@@ -36298,7 +36291,7 @@
         <v>261</v>
       </c>
       <c r="S431" s="55" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="T431" s="55"/>
     </row>
@@ -36529,14 +36522,14 @@
         <v>967</v>
       </c>
       <c r="P436" s="183" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="Q436" s="10"/>
       <c r="R436" s="158" t="s">
         <v>1246</v>
       </c>
       <c r="S436" s="55" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="T436" s="10"/>
     </row>
@@ -36592,7 +36585,7 @@
         <v>263</v>
       </c>
       <c r="S437" s="182" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="T437" s="55"/>
     </row>
@@ -36659,7 +36652,7 @@
         <v>carbon-capture-and-sequestration.html</v>
       </c>
       <c r="S438" s="182" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="T438" s="55"/>
     </row>
@@ -36716,7 +36709,7 @@
         <v>265</v>
       </c>
       <c r="S439" s="10" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="T439" s="10"/>
     </row>
@@ -36783,7 +36776,7 @@
         <v>carbon-tax.html</v>
       </c>
       <c r="S440" s="57" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="T440" s="57"/>
     </row>
@@ -36850,7 +36843,7 @@
         <v>carbon-tax.html</v>
       </c>
       <c r="S441" s="57" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="T441" s="57"/>
     </row>
@@ -36917,7 +36910,7 @@
         <v>carbon-tax.html</v>
       </c>
       <c r="S442" s="57" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="T442" s="57"/>
     </row>
@@ -36984,7 +36977,7 @@
         <v>carbon-tax.html</v>
       </c>
       <c r="S443" s="57" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="T443" s="57"/>
     </row>
@@ -37122,7 +37115,7 @@
         <v>265</v>
       </c>
       <c r="S446" s="57" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="T446" s="10"/>
     </row>
@@ -37283,7 +37276,7 @@
         <v>269</v>
       </c>
       <c r="S449" s="55" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="T449" s="57"/>
     </row>
@@ -38046,7 +38039,7 @@
       <c r="Q465" s="57"/>
       <c r="R465" s="158"/>
       <c r="S465" s="76" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="T465" s="57"/>
     </row>
@@ -38992,7 +38985,7 @@
         <v>271</v>
       </c>
       <c r="S487" s="55" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="T487" s="57"/>
     </row>
@@ -44043,21 +44036,21 @@
       <c r="M571" s="389">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="N571" s="402">
+      <c r="N571" s="393">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="O571" s="4" t="s">
         <v>1434</v>
       </c>
-      <c r="P571" s="2" t="s">
-        <v>1629</v>
+      <c r="P571" s="403" t="s">
+        <v>1963</v>
       </c>
       <c r="R571" s="162"/>
       <c r="S571" s="67" t="s">
+        <v>1675</v>
+      </c>
+      <c r="T571" s="2" t="s">
         <v>1676</v>
-      </c>
-      <c r="T571" s="2" t="s">
-        <v>1677</v>
       </c>
     </row>
     <row r="572" spans="1:20">
@@ -44528,10 +44521,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="393" t="s">
+      <c r="A1" s="394" t="s">
         <v>1415</v>
       </c>
-      <c r="B1" s="393"/>
+      <c r="B1" s="394"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="166" t="s">
@@ -44555,7 +44548,7 @@
         <v>1425</v>
       </c>
       <c r="B4" s="193" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -44572,7 +44565,7 @@
         <v>1426</v>
       </c>
       <c r="B6" s="193" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -44580,7 +44573,7 @@
         <v>828</v>
       </c>
       <c r="B7" s="193" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -44588,7 +44581,7 @@
         <v>829</v>
       </c>
       <c r="B8" s="193" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -44623,7 +44616,7 @@
         <v>830</v>
       </c>
       <c r="B12" s="193" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -44640,7 +44633,7 @@
         <v>817</v>
       </c>
       <c r="B14" s="193" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -44648,7 +44641,7 @@
         <v>818</v>
       </c>
       <c r="B15" s="193" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -44692,7 +44685,7 @@
         <v>512</v>
       </c>
       <c r="B20" s="193" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -44700,7 +44693,7 @@
         <v>1424</v>
       </c>
       <c r="B21" s="193" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -44708,7 +44701,7 @@
         <v>800</v>
       </c>
       <c r="B22" s="193" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -44716,7 +44709,7 @@
         <v>801</v>
       </c>
       <c r="B23" s="193" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -44724,7 +44717,7 @@
         <v>724</v>
       </c>
       <c r="B24" s="193" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -44732,7 +44725,7 @@
         <v>1144</v>
       </c>
       <c r="B25" s="193" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -44749,7 +44742,7 @@
         <v>831</v>
       </c>
       <c r="B27" s="193" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -44757,7 +44750,7 @@
         <v>832</v>
       </c>
       <c r="B28" s="193" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -44765,7 +44758,7 @@
         <v>833</v>
       </c>
       <c r="B29" s="193" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -44773,7 +44766,7 @@
         <v>1177</v>
       </c>
       <c r="B30" s="194" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -44781,7 +44774,7 @@
         <v>1178</v>
       </c>
       <c r="B31" s="194" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -44789,7 +44782,7 @@
         <v>834</v>
       </c>
       <c r="B32" s="193" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -44797,7 +44790,7 @@
         <v>839</v>
       </c>
       <c r="B33" s="193" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -44805,7 +44798,7 @@
         <v>866</v>
       </c>
       <c r="B34" s="193" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -44813,14 +44806,14 @@
         <v>973</v>
       </c>
       <c r="B35" s="193" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="393" t="s">
+      <c r="A37" s="394" t="s">
         <v>1419</v>
       </c>
-      <c r="B37" s="393"/>
+      <c r="B37" s="394"/>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="166" t="s">
@@ -44835,7 +44828,7 @@
         <v>160</v>
       </c>
       <c r="B39" s="193" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -44843,7 +44836,7 @@
         <v>162</v>
       </c>
       <c r="B40" s="193" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="51" spans="1:1">
@@ -46725,7 +46718,7 @@
         <v>793</v>
       </c>
       <c r="H68" s="380" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="I68" s="96" t="s">
         <v>1073</v>
@@ -46752,13 +46745,13 @@
         <v>trillion freight ton-km / year</v>
       </c>
       <c r="G69" s="381" t="s">
+        <v>1926</v>
+      </c>
+      <c r="H69" s="382" t="s">
         <v>1927</v>
       </c>
-      <c r="H69" s="382" t="s">
+      <c r="I69" s="381" t="s">
         <v>1928</v>
-      </c>
-      <c r="I69" s="381" t="s">
-        <v>1929</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="71.25">
@@ -46812,13 +46805,13 @@
         <v>thousand vehicles / year</v>
       </c>
       <c r="G71" s="383" t="s">
+        <v>1929</v>
+      </c>
+      <c r="H71" s="383" t="s">
         <v>1930</v>
       </c>
-      <c r="H71" s="383" t="s">
+      <c r="I71" s="383" t="s">
         <v>1931</v>
-      </c>
-      <c r="I71" s="383" t="s">
-        <v>1932</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="42.75">
@@ -46842,13 +46835,13 @@
         <v>thousand vehicles / year</v>
       </c>
       <c r="G72" s="383" t="s">
+        <v>1932</v>
+      </c>
+      <c r="H72" s="383" t="s">
         <v>1933</v>
       </c>
-      <c r="H72" s="383" t="s">
+      <c r="I72" s="383" t="s">
         <v>1934</v>
-      </c>
-      <c r="I72" s="383" t="s">
-        <v>1935</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="42.75">
@@ -46872,13 +46865,13 @@
         <v>thousand vehicles / year</v>
       </c>
       <c r="G73" s="383" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="H73" s="383" t="s">
+        <v>1933</v>
+      </c>
+      <c r="I73" s="383" t="s">
         <v>1934</v>
-      </c>
-      <c r="I73" s="383" t="s">
-        <v>1935</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="28.5">
@@ -46886,7 +46879,7 @@
         <v>1313</v>
       </c>
       <c r="B74" s="384" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="C74" s="164">
         <v>1</v>
@@ -46916,7 +46909,7 @@
         <v>1313</v>
       </c>
       <c r="B75" s="384" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="C75" s="385">
         <v>1</v>
@@ -46931,13 +46924,13 @@
         <v>795</v>
       </c>
       <c r="G75" s="383" t="s">
+        <v>1938</v>
+      </c>
+      <c r="H75" s="383" t="s">
         <v>1939</v>
       </c>
-      <c r="H75" s="383" t="s">
+      <c r="I75" s="383" t="s">
         <v>1940</v>
-      </c>
-      <c r="I75" s="383" t="s">
-        <v>1941</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="57">
@@ -46991,13 +46984,13 @@
         <v>thousand vehicles</v>
       </c>
       <c r="G77" s="383" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="H77" s="383" t="s">
+        <v>1930</v>
+      </c>
+      <c r="I77" s="383" t="s">
         <v>1931</v>
-      </c>
-      <c r="I77" s="383" t="s">
-        <v>1932</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="42.75">
@@ -47021,13 +47014,13 @@
         <v>million vehicles</v>
       </c>
       <c r="G78" s="383" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="H78" s="383" t="s">
+        <v>1933</v>
+      </c>
+      <c r="I78" s="383" t="s">
         <v>1934</v>
-      </c>
-      <c r="I78" s="383" t="s">
-        <v>1935</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="42.75">
@@ -47051,13 +47044,13 @@
         <v>million vehicles</v>
       </c>
       <c r="G79" s="383" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="H79" s="383" t="s">
+        <v>1933</v>
+      </c>
+      <c r="I79" s="383" t="s">
         <v>1934</v>
-      </c>
-      <c r="I79" s="383" t="s">
-        <v>1935</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="28.9" thickBot="1">
@@ -47065,7 +47058,7 @@
         <v>1313</v>
       </c>
       <c r="B80" s="386" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="C80" s="171">
         <v>1</v>
@@ -47095,7 +47088,7 @@
         <v>1313</v>
       </c>
       <c r="B81" s="386" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="C81" s="387">
         <v>1</v>
@@ -47110,13 +47103,13 @@
         <v>794</v>
       </c>
       <c r="G81" s="383" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="H81" s="383" t="s">
+        <v>1939</v>
+      </c>
+      <c r="I81" s="383" t="s">
         <v>1940</v>
-      </c>
-      <c r="I81" s="383" t="s">
-        <v>1941</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="128.25">
@@ -47140,13 +47133,13 @@
         <v>million metric tons / year</v>
       </c>
       <c r="G82" s="383" t="s">
+        <v>1947</v>
+      </c>
+      <c r="H82" s="383" t="s">
         <v>1948</v>
       </c>
-      <c r="H82" s="383" t="s">
+      <c r="I82" s="383" t="s">
         <v>1949</v>
-      </c>
-      <c r="I82" s="383" t="s">
-        <v>1950</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="85.5">
@@ -47200,13 +47193,13 @@
         <v>petajoules / year</v>
       </c>
       <c r="G84" s="383" t="s">
+        <v>1950</v>
+      </c>
+      <c r="H84" s="383" t="s">
+        <v>1948</v>
+      </c>
+      <c r="I84" s="381" t="s">
         <v>1951</v>
-      </c>
-      <c r="H84" s="383" t="s">
-        <v>1949</v>
-      </c>
-      <c r="I84" s="381" t="s">
-        <v>1952</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="57">
@@ -50910,18 +50903,18 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="9" t="s">
+        <v>1959</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>1960</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>1961</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="9" t="s">
+        <v>1961</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>1962</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>1963</v>
       </c>
     </row>
   </sheetData>
@@ -50982,7 +50975,7 @@
         <v>5382.9603750904134</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -50991,7 +50984,7 @@
     </row>
     <row r="4" spans="1:5" s="95" customFormat="1">
       <c r="A4" s="1" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="B4" s="168"/>
       <c r="C4" s="378"/>
@@ -51000,7 +50993,7 @@
     </row>
     <row r="5" spans="1:5" s="95" customFormat="1">
       <c r="A5" s="25" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="6"/>
@@ -51009,7 +51002,7 @@
     </row>
     <row r="6" spans="1:5" s="95" customFormat="1">
       <c r="A6" s="25" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="6"/>
@@ -51018,7 +51011,7 @@
     </row>
     <row r="7" spans="1:5" s="95" customFormat="1">
       <c r="A7" s="25" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="6"/>
@@ -51034,7 +51027,7 @@
     </row>
     <row r="9" spans="1:5" s="95" customFormat="1">
       <c r="A9" s="25" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="6"/>
@@ -51043,7 +51036,7 @@
     </row>
     <row r="10" spans="1:5" s="95" customFormat="1">
       <c r="A10" s="25" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="6"/>
@@ -51059,7 +51052,7 @@
     </row>
     <row r="12" spans="1:5" s="95" customFormat="1">
       <c r="A12" s="25" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="6"/>
@@ -51068,7 +51061,7 @@
     </row>
     <row r="13" spans="1:5" s="95" customFormat="1">
       <c r="A13" s="25" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="6"/>
@@ -51077,7 +51070,7 @@
     </row>
     <row r="14" spans="1:5" s="95" customFormat="1">
       <c r="A14" s="25" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="6"/>
@@ -51086,7 +51079,7 @@
     </row>
     <row r="15" spans="1:5" s="95" customFormat="1">
       <c r="A15" s="25" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="6"/>
@@ -51095,7 +51088,7 @@
     </row>
     <row r="16" spans="1:5" s="95" customFormat="1">
       <c r="A16" s="49" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="6"/>
@@ -51111,7 +51104,7 @@
     </row>
     <row r="18" spans="1:5" s="95" customFormat="1">
       <c r="A18" s="25" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="6"/>
@@ -51120,7 +51113,7 @@
     </row>
     <row r="19" spans="1:5" s="95" customFormat="1">
       <c r="A19" s="25" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="6"/>
@@ -51129,7 +51122,7 @@
     </row>
     <row r="20" spans="1:5" s="95" customFormat="1">
       <c r="A20" s="25" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="6"/>
@@ -51138,7 +51131,7 @@
     </row>
     <row r="21" spans="1:5" s="95" customFormat="1">
       <c r="A21" s="25" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="6"/>
@@ -51147,7 +51140,7 @@
     </row>
     <row r="22" spans="1:5" s="95" customFormat="1">
       <c r="A22" s="25" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="6"/>
@@ -51163,7 +51156,7 @@
     </row>
     <row r="24" spans="1:5" s="95" customFormat="1">
       <c r="A24" s="21" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="6"/>
@@ -51172,7 +51165,7 @@
     </row>
     <row r="25" spans="1:5" s="95" customFormat="1">
       <c r="A25" s="25" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="6"/>
@@ -51181,7 +51174,7 @@
     </row>
     <row r="26" spans="1:5" s="95" customFormat="1">
       <c r="A26" s="25" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="6"/>
@@ -51204,7 +51197,7 @@
     </row>
     <row r="29" spans="1:5" s="95" customFormat="1">
       <c r="A29" s="50" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="6"/>
@@ -51213,7 +51206,7 @@
     </row>
     <row r="30" spans="1:5" s="95" customFormat="1">
       <c r="A30" s="25" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="6"/>
@@ -51231,7 +51224,7 @@
     </row>
     <row r="32" spans="1:5" s="95" customFormat="1">
       <c r="A32" s="95" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="6"/>
@@ -51240,7 +51233,7 @@
     </row>
     <row r="33" spans="1:5" s="95" customFormat="1">
       <c r="A33" s="49" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="6"/>
@@ -51249,7 +51242,7 @@
     </row>
     <row r="34" spans="1:5" s="95" customFormat="1">
       <c r="A34" s="25" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="6"/>
@@ -51265,7 +51258,7 @@
     </row>
     <row r="36" spans="1:5" s="95" customFormat="1">
       <c r="A36" s="50" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="6"/>
@@ -51274,7 +51267,7 @@
     </row>
     <row r="37" spans="1:5" s="95" customFormat="1">
       <c r="A37" s="25" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="6"/>
@@ -51292,7 +51285,7 @@
     </row>
     <row r="39" spans="1:5" s="95" customFormat="1">
       <c r="A39" s="95" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="6"/>
@@ -51301,7 +51294,7 @@
     </row>
     <row r="40" spans="1:5" s="95" customFormat="1">
       <c r="A40" s="49" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="6"/>
@@ -51310,7 +51303,7 @@
     </row>
     <row r="41" spans="1:5" s="95" customFormat="1">
       <c r="A41" s="25" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="6"/>
@@ -51326,7 +51319,7 @@
     </row>
     <row r="43" spans="1:5" s="95" customFormat="1">
       <c r="A43" s="50" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="6"/>
@@ -51335,7 +51328,7 @@
     </row>
     <row r="44" spans="1:5" s="95" customFormat="1">
       <c r="A44" s="95" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="6"/>
@@ -51353,7 +51346,7 @@
     </row>
     <row r="46" spans="1:5" s="95" customFormat="1">
       <c r="A46" s="95" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="B46" s="4"/>
       <c r="C46" s="6"/>
@@ -51362,7 +51355,7 @@
     </row>
     <row r="47" spans="1:5" s="95" customFormat="1">
       <c r="A47" s="49" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="6"/>
@@ -51371,7 +51364,7 @@
     </row>
     <row r="48" spans="1:5" s="95" customFormat="1">
       <c r="A48" s="25" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="6"/>
@@ -51387,7 +51380,7 @@
     </row>
     <row r="50" spans="1:5" s="95" customFormat="1">
       <c r="A50" s="50" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="6"/>
@@ -51396,7 +51389,7 @@
     </row>
     <row r="51" spans="1:5" s="95" customFormat="1">
       <c r="A51" s="25" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="6"/>
@@ -51414,7 +51407,7 @@
     </row>
     <row r="53" spans="1:5" s="95" customFormat="1">
       <c r="A53" s="25" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="B53" s="4"/>
       <c r="C53" s="6"/>
@@ -51423,7 +51416,7 @@
     </row>
     <row r="54" spans="1:5" s="95" customFormat="1">
       <c r="A54" s="49" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="B54" s="4"/>
       <c r="C54" s="6"/>
@@ -51432,7 +51425,7 @@
     </row>
     <row r="55" spans="1:5" s="95" customFormat="1">
       <c r="A55" s="25" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="B55" s="4"/>
       <c r="C55" s="6"/>
@@ -51455,7 +51448,7 @@
     </row>
     <row r="58" spans="1:5" s="95" customFormat="1">
       <c r="A58" s="50" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="B58" s="168"/>
       <c r="C58" s="378"/>
@@ -51464,13 +51457,13 @@
     </row>
     <row r="59" spans="1:5" s="95" customFormat="1" ht="28.5">
       <c r="A59" s="115" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="B59" s="377" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="C59" s="377" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="4"/>
@@ -51641,7 +51634,7 @@
     <row r="73" spans="1:7" s="95" customFormat="1"/>
     <row r="74" spans="1:7" s="95" customFormat="1" ht="15.75">
       <c r="A74" s="343" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="B74" s="376"/>
       <c r="C74" s="376"/>
@@ -51652,10 +51645,10 @@
     <row r="75" spans="1:7" s="95" customFormat="1" ht="28.5">
       <c r="A75" s="375"/>
       <c r="B75" s="374" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="C75" s="374" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="D75" s="374" t="s">
         <v>569</v>
@@ -51664,13 +51657,13 @@
         <v>570</v>
       </c>
       <c r="F75" s="373" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="G75" s="110"/>
     </row>
     <row r="76" spans="1:7" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A76" s="372" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="B76" s="371">
         <v>1497029.2</v>
@@ -51690,7 +51683,7 @@
     </row>
     <row r="77" spans="1:7" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A77" s="358" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="B77" s="355">
         <v>992836.3</v>
@@ -51708,7 +51701,7 @@
     </row>
     <row r="78" spans="1:7" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A78" s="354" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="B78" s="350">
         <v>715829.8</v>
@@ -51726,7 +51719,7 @@
     </row>
     <row r="79" spans="1:7" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A79" s="354" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="B79" s="350">
         <v>33787.5</v>
@@ -51744,7 +51737,7 @@
     </row>
     <row r="80" spans="1:7" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A80" s="354" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="B80" s="350">
         <v>138858</v>
@@ -51762,7 +51755,7 @@
     </row>
     <row r="81" spans="1:7" s="95" customFormat="1">
       <c r="A81" s="370" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="B81" s="369">
         <v>121211</v>
@@ -51780,7 +51773,7 @@
     </row>
     <row r="82" spans="1:7" s="95" customFormat="1">
       <c r="A82" s="370" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="B82" s="369">
         <v>6109</v>
@@ -51852,7 +51845,7 @@
     </row>
     <row r="86" spans="1:7" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A86" s="354" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="B86" s="350">
         <v>1657</v>
@@ -51870,7 +51863,7 @@
     </row>
     <row r="87" spans="1:7" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A87" s="354" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="B87" s="350">
         <v>33277</v>
@@ -51902,7 +51895,7 @@
     </row>
     <row r="89" spans="1:7" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A89" s="358" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="B89" s="355">
         <v>405862.9</v>
@@ -51921,7 +51914,7 @@
     </row>
     <row r="90" spans="1:7" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A90" s="368" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="B90" s="366">
         <v>130783.95</v>
@@ -51939,7 +51932,7 @@
     </row>
     <row r="91" spans="1:7" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A91" s="354" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="B91" s="350">
         <v>129920</v>
@@ -51953,7 +51946,7 @@
     </row>
     <row r="92" spans="1:7" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A92" s="354" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="B92" s="350">
         <v>277.82</v>
@@ -51971,7 +51964,7 @@
     </row>
     <row r="93" spans="1:7" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A93" s="354" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="B93" s="350">
         <v>586.12</v>
@@ -52003,7 +51996,7 @@
     </row>
     <row r="95" spans="1:7" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A95" s="354" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="B95" s="350">
         <v>10056.43</v>
@@ -52017,7 +52010,7 @@
     </row>
     <row r="96" spans="1:7" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A96" s="354" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="B96" s="352"/>
       <c r="C96" s="352"/>
@@ -52031,7 +52024,7 @@
     </row>
     <row r="97" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A97" s="354" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="B97" s="350">
         <v>119.58</v>
@@ -52045,7 +52038,7 @@
     </row>
     <row r="98" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A98" s="354" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="B98" s="350">
         <v>88.04</v>
@@ -52059,7 +52052,7 @@
     </row>
     <row r="99" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A99" s="354" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="B99" s="350">
         <v>266.18</v>
@@ -52075,7 +52068,7 @@
     </row>
     <row r="100" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A100" s="354" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="B100" s="350">
         <v>7072.52</v>
@@ -52091,7 +52084,7 @@
     </row>
     <row r="101" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A101" s="354" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="B101" s="350">
         <v>198.91</v>
@@ -52105,7 +52098,7 @@
     </row>
     <row r="102" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A102" s="354" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="B102" s="350">
         <v>93.64</v>
@@ -52121,7 +52114,7 @@
     </row>
     <row r="103" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A103" s="354" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="B103" s="350">
         <v>37.840000000000003</v>
@@ -52137,7 +52130,7 @@
     </row>
     <row r="104" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A104" s="354" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="B104" s="350">
         <v>1155.52</v>
@@ -52153,7 +52146,7 @@
     </row>
     <row r="105" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A105" s="354" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="B105" s="352"/>
       <c r="C105" s="352"/>
@@ -52167,7 +52160,7 @@
     </row>
     <row r="106" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A106" s="354" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="B106" s="350">
         <v>8800.2099999999991</v>
@@ -52185,7 +52178,7 @@
     </row>
     <row r="107" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A107" s="368" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="B107" s="366">
         <v>122371.43</v>
@@ -52203,7 +52196,7 @@
     </row>
     <row r="108" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A108" s="354" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="B108" s="350">
         <v>116958.37</v>
@@ -52221,7 +52214,7 @@
     </row>
     <row r="109" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A109" s="354" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="B109" s="350">
         <v>2460.6999999999998</v>
@@ -52237,7 +52230,7 @@
     </row>
     <row r="110" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A110" s="354" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="B110" s="350">
         <v>2728.87</v>
@@ -52255,7 +52248,7 @@
     </row>
     <row r="111" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A111" s="354" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="B111" s="350">
         <v>84.13</v>
@@ -52273,7 +52266,7 @@
     </row>
     <row r="112" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A112" s="354" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="B112" s="350">
         <v>76.11</v>
@@ -52291,7 +52284,7 @@
     </row>
     <row r="113" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A113" s="354" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="B113" s="350">
         <v>63.25</v>
@@ -52327,7 +52320,7 @@
     </row>
     <row r="115" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A115" s="354" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="B115" s="350">
         <v>5222.5</v>
@@ -52345,7 +52338,7 @@
     </row>
     <row r="116" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A116" s="354" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="B116" s="350">
         <v>27625.53</v>
@@ -52363,7 +52356,7 @@
     </row>
     <row r="117" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A117" s="354" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="B117" s="350">
         <v>1861.11</v>
@@ -52381,7 +52374,7 @@
     </row>
     <row r="118" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A118" s="354" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="B118" s="350">
         <v>1460.26</v>
@@ -52399,7 +52392,7 @@
     </row>
     <row r="119" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A119" s="354" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="B119" s="350">
         <v>87799.77</v>
@@ -52417,7 +52410,7 @@
     </row>
     <row r="120" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A120" s="365" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="B120" s="364">
         <v>849.49</v>
@@ -52431,7 +52424,7 @@
     </row>
     <row r="121" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A121" s="354" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="B121" s="350">
         <v>776.75</v>
@@ -52445,7 +52438,7 @@
     </row>
     <row r="122" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A122" s="354" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="B122" s="350">
         <v>72.75</v>
@@ -52459,7 +52452,7 @@
     </row>
     <row r="123" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A123" s="358" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="B123" s="356"/>
       <c r="C123" s="356"/>
@@ -52475,7 +52468,7 @@
     </row>
     <row r="124" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A124" s="354" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="B124" s="352"/>
       <c r="C124" s="352"/>
@@ -52489,7 +52482,7 @@
     </row>
     <row r="125" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A125" s="354" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="B125" s="352"/>
       <c r="C125" s="352"/>
@@ -52505,7 +52498,7 @@
     </row>
     <row r="126" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A126" s="354" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="B126" s="352"/>
       <c r="C126" s="352"/>
@@ -52519,7 +52512,7 @@
     </row>
     <row r="127" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A127" s="354" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="B127" s="352"/>
       <c r="C127" s="352"/>
@@ -52533,7 +52526,7 @@
     </row>
     <row r="128" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A128" s="354" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="B128" s="352"/>
       <c r="C128" s="352"/>
@@ -52549,7 +52542,7 @@
     </row>
     <row r="129" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A129" s="358" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="B129" s="355">
         <v>98330</v>
@@ -52565,7 +52558,7 @@
     </row>
     <row r="130" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A130" s="354" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="B130" s="352"/>
       <c r="C130" s="350">
@@ -52579,7 +52572,7 @@
     </row>
     <row r="131" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A131" s="354" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="B131" s="352"/>
       <c r="C131" s="350">
@@ -52593,7 +52586,7 @@
     </row>
     <row r="132" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A132" s="354" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="B132" s="350">
         <v>10490</v>
@@ -52607,7 +52600,7 @@
     </row>
     <row r="133" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A133" s="354" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="B133" s="352"/>
       <c r="C133" s="350">
@@ -52621,7 +52614,7 @@
     </row>
     <row r="134" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A134" s="354" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="B134" s="359" t="s">
         <v>543</v>
@@ -52635,7 +52628,7 @@
     </row>
     <row r="135" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A135" s="354" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="B135" s="354" t="s">
         <v>544</v>
@@ -52649,7 +52642,7 @@
     </row>
     <row r="136" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A136" s="354" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="B136" s="350">
         <v>87840</v>
@@ -52663,7 +52656,7 @@
     </row>
     <row r="137" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A137" s="358" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="B137" s="356"/>
       <c r="C137" s="356"/>
@@ -52679,7 +52672,7 @@
     </row>
     <row r="138" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A138" s="354" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="B138" s="352"/>
       <c r="C138" s="352"/>
@@ -52693,7 +52686,7 @@
     </row>
     <row r="139" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A139" s="354" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="B139" s="352"/>
       <c r="C139" s="352"/>
@@ -52709,7 +52702,7 @@
     </row>
     <row r="140" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A140" s="354" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="B140" s="352"/>
       <c r="C140" s="352"/>
@@ -52723,7 +52716,7 @@
     </row>
     <row r="141" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A141" s="358" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="B141" s="357">
         <v>3454</v>
@@ -52741,7 +52734,7 @@
     </row>
     <row r="142" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A142" s="354" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="B142" s="353">
         <v>3326</v>
@@ -52759,7 +52752,7 @@
     </row>
     <row r="143" spans="1:6" s="95" customFormat="1" ht="16.149999999999999">
       <c r="A143" s="354" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="B143" s="353">
         <v>128</v>
@@ -52777,7 +52770,7 @@
     </row>
     <row r="144" spans="1:6" s="95" customFormat="1">
       <c r="A144" s="349" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="B144" s="83"/>
       <c r="C144" s="83"/>
@@ -52787,7 +52780,7 @@
     </row>
     <row r="145" spans="1:11" s="95" customFormat="1">
       <c r="A145" s="349" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="B145" s="83"/>
       <c r="C145" s="83"/>
@@ -52811,7 +52804,7 @@
     </row>
     <row r="147" spans="1:11" s="95" customFormat="1">
       <c r="A147" s="319" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="B147" s="347">
         <f>B76-C76</f>
@@ -52830,7 +52823,7 @@
     </row>
     <row r="148" spans="1:11" s="95" customFormat="1">
       <c r="A148" s="319" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="B148" s="83">
         <f>B147*$C$60</f>
@@ -52849,7 +52842,7 @@
     </row>
     <row r="149" spans="1:11" s="95" customFormat="1">
       <c r="A149" s="319" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="B149" s="83">
         <f>SUM(B148:E148)</f>
@@ -52871,7 +52864,7 @@
     <row r="151" spans="1:11" s="95" customFormat="1"/>
     <row r="152" spans="1:11" s="95" customFormat="1" ht="15" customHeight="1">
       <c r="A152" s="344" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="B152" s="343"/>
       <c r="C152" s="343"/>
@@ -52887,10 +52880,10 @@
     <row r="153" spans="1:11" s="95" customFormat="1" ht="40.5">
       <c r="A153" s="341"/>
       <c r="B153" s="341" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="C153" s="341" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="D153" s="341" t="s">
         <v>569</v>
@@ -52914,12 +52907,12 @@
         <v>559</v>
       </c>
       <c r="K153" s="341" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="154" spans="1:11" s="95" customFormat="1">
       <c r="A154" s="340" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="B154" s="337">
         <v>1024772.84</v>
@@ -52954,7 +52947,7 @@
     </row>
     <row r="155" spans="1:11" s="95" customFormat="1">
       <c r="A155" s="327" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="B155" s="328">
         <v>952212.06</v>
@@ -52977,7 +52970,7 @@
     </row>
     <row r="156" spans="1:11" s="95" customFormat="1">
       <c r="A156" s="334" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="B156" s="321">
         <v>952212.06</v>
@@ -53023,7 +53016,7 @@
     </row>
     <row r="158" spans="1:11" s="95" customFormat="1">
       <c r="A158" s="325" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="B158" s="321">
         <v>522495.43</v>
@@ -53046,7 +53039,7 @@
     </row>
     <row r="159" spans="1:11" s="95" customFormat="1">
       <c r="A159" s="325" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="B159" s="321">
         <v>18695.900000000001</v>
@@ -53069,10 +53062,10 @@
     </row>
     <row r="160" spans="1:11" s="95" customFormat="1" ht="27">
       <c r="A160" s="325" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="B160" s="325" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C160" s="322"/>
       <c r="D160" s="325" t="s">
@@ -53115,7 +53108,7 @@
     </row>
     <row r="162" spans="1:11" s="95" customFormat="1">
       <c r="A162" s="325" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="B162" s="321">
         <v>39696</v>
@@ -53134,7 +53127,7 @@
     </row>
     <row r="163" spans="1:11" s="95" customFormat="1">
       <c r="A163" s="325" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="B163" s="321">
         <v>52366.02</v>
@@ -53157,7 +53150,7 @@
     </row>
     <row r="164" spans="1:11" s="95" customFormat="1">
       <c r="A164" s="325" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="B164" s="321">
         <v>1885.88</v>
@@ -53180,7 +53173,7 @@
     </row>
     <row r="165" spans="1:11" s="95" customFormat="1">
       <c r="A165" s="325" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="B165" s="321">
         <v>34482.44</v>
@@ -53203,7 +53196,7 @@
     </row>
     <row r="166" spans="1:11" s="95" customFormat="1">
       <c r="A166" s="325" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="B166" s="321">
         <v>5331.75</v>
@@ -53226,7 +53219,7 @@
     </row>
     <row r="167" spans="1:11" s="95" customFormat="1">
       <c r="A167" s="325" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="B167" s="321">
         <v>24577.85</v>
@@ -53249,7 +53242,7 @@
     </row>
     <row r="168" spans="1:11" s="95" customFormat="1">
       <c r="A168" s="325" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="B168" s="321">
         <v>1010.93</v>
@@ -53272,7 +53265,7 @@
     </row>
     <row r="169" spans="1:11" s="95" customFormat="1">
       <c r="A169" s="325" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="B169" s="321">
         <v>2509.79</v>
@@ -53295,7 +53288,7 @@
     </row>
     <row r="170" spans="1:11" s="95" customFormat="1">
       <c r="A170" s="325" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="B170" s="321">
         <v>7669.09</v>
@@ -53318,7 +53311,7 @@
     </row>
     <row r="171" spans="1:11" s="95" customFormat="1">
       <c r="A171" s="325" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="B171" s="321">
         <v>58717.17</v>
@@ -53364,7 +53357,7 @@
     </row>
     <row r="173" spans="1:11" s="95" customFormat="1">
       <c r="A173" s="325" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="B173" s="321">
         <v>85515.82</v>
@@ -53387,7 +53380,7 @@
     </row>
     <row r="174" spans="1:11" s="95" customFormat="1">
       <c r="A174" s="325" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="B174" s="321">
         <v>4021.98</v>
@@ -53410,7 +53403,7 @@
     </row>
     <row r="175" spans="1:11" s="95" customFormat="1">
       <c r="A175" s="325" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="B175" s="321">
         <v>5426.32</v>
@@ -53433,7 +53426,7 @@
     </row>
     <row r="176" spans="1:11" s="95" customFormat="1">
       <c r="A176" s="325" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="B176" s="321">
         <v>1012.71</v>
@@ -53479,7 +53472,7 @@
     </row>
     <row r="178" spans="1:11" s="95" customFormat="1">
       <c r="A178" s="325" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="B178" s="321">
         <v>3268</v>
@@ -53502,7 +53495,7 @@
     </row>
     <row r="179" spans="1:11" s="95" customFormat="1">
       <c r="A179" s="325" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="B179" s="321">
         <v>55182</v>
@@ -53525,7 +53518,7 @@
     </row>
     <row r="180" spans="1:11" s="95" customFormat="1">
       <c r="A180" s="325" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="B180" s="321">
         <v>28347</v>
@@ -53548,7 +53541,7 @@
     </row>
     <row r="181" spans="1:11" s="95" customFormat="1">
       <c r="A181" s="334" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="B181" s="322"/>
       <c r="C181" s="322"/>
@@ -53586,7 +53579,7 @@
     </row>
     <row r="183" spans="1:11" s="95" customFormat="1">
       <c r="A183" s="325" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="B183" s="322"/>
       <c r="C183" s="322"/>
@@ -53605,7 +53598,7 @@
     </row>
     <row r="184" spans="1:11" s="95" customFormat="1">
       <c r="A184" s="325" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="B184" s="322"/>
       <c r="C184" s="322"/>
@@ -53624,7 +53617,7 @@
     </row>
     <row r="185" spans="1:11" s="95" customFormat="1">
       <c r="A185" s="334" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="B185" s="322"/>
       <c r="C185" s="322"/>
@@ -53643,7 +53636,7 @@
     </row>
     <row r="186" spans="1:11" s="95" customFormat="1">
       <c r="A186" s="325" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="B186" s="322"/>
       <c r="C186" s="322"/>
@@ -53662,7 +53655,7 @@
     </row>
     <row r="187" spans="1:11" s="95" customFormat="1">
       <c r="A187" s="325" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B187" s="322"/>
       <c r="C187" s="322"/>
@@ -53681,7 +53674,7 @@
     </row>
     <row r="188" spans="1:11" s="95" customFormat="1">
       <c r="A188" s="325" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B188" s="322"/>
       <c r="C188" s="322"/>
@@ -53700,7 +53693,7 @@
     </row>
     <row r="189" spans="1:11" s="95" customFormat="1">
       <c r="A189" s="327" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="B189" s="328">
         <v>72560.78</v>
@@ -53733,7 +53726,7 @@
     </row>
     <row r="190" spans="1:11" s="95" customFormat="1">
       <c r="A190" s="334" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="B190" s="321">
         <v>53558.17</v>
@@ -53752,7 +53745,7 @@
     </row>
     <row r="191" spans="1:11" s="95" customFormat="1">
       <c r="A191" s="325" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="B191" s="321">
         <v>44056</v>
@@ -53771,7 +53764,7 @@
     </row>
     <row r="192" spans="1:11" s="95" customFormat="1">
       <c r="A192" s="325" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="B192" s="321">
         <v>2921</v>
@@ -53790,7 +53783,7 @@
     </row>
     <row r="193" spans="1:11" s="95" customFormat="1">
       <c r="A193" s="325" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="B193" s="321">
         <v>5961.68</v>
@@ -53809,7 +53802,7 @@
     </row>
     <row r="194" spans="1:11" s="95" customFormat="1">
       <c r="A194" s="325" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="B194" s="323">
         <v>463.94</v>
@@ -53828,7 +53821,7 @@
     </row>
     <row r="195" spans="1:11" s="95" customFormat="1">
       <c r="A195" s="325" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="B195" s="323">
         <v>155.54</v>
@@ -53847,7 +53840,7 @@
     </row>
     <row r="196" spans="1:11" s="95" customFormat="1">
       <c r="A196" s="334" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="B196" s="321">
         <v>15785.98</v>
@@ -53870,7 +53863,7 @@
     </row>
     <row r="197" spans="1:11" s="95" customFormat="1">
       <c r="A197" s="325" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="B197" s="321">
         <v>11067.3</v>
@@ -53889,7 +53882,7 @@
     </row>
     <row r="198" spans="1:11" s="95" customFormat="1">
       <c r="A198" s="325" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="B198" s="323">
         <v>0</v>
@@ -53910,7 +53903,7 @@
     </row>
     <row r="199" spans="1:11" s="95" customFormat="1">
       <c r="A199" s="325" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="B199" s="323">
         <v>102.72</v>
@@ -53929,7 +53922,7 @@
     </row>
     <row r="200" spans="1:11" s="95" customFormat="1">
       <c r="A200" s="325" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="B200" s="323">
         <v>43.75</v>
@@ -53948,7 +53941,7 @@
     </row>
     <row r="201" spans="1:11" s="95" customFormat="1">
       <c r="A201" s="325" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="B201" s="323">
         <v>229.84</v>
@@ -53969,7 +53962,7 @@
     </row>
     <row r="202" spans="1:11" s="95" customFormat="1">
       <c r="A202" s="325" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="B202" s="321">
         <v>3317.23</v>
@@ -53990,7 +53983,7 @@
     </row>
     <row r="203" spans="1:11" s="95" customFormat="1">
       <c r="A203" s="325" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="B203" s="323">
         <v>233.23</v>
@@ -54009,7 +54002,7 @@
     </row>
     <row r="204" spans="1:11" s="95" customFormat="1">
       <c r="A204" s="325" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="B204" s="323">
         <v>51.29</v>
@@ -54030,7 +54023,7 @@
     </row>
     <row r="205" spans="1:11" s="95" customFormat="1">
       <c r="A205" s="325" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="B205" s="323">
         <v>26.98</v>
@@ -54051,7 +54044,7 @@
     </row>
     <row r="206" spans="1:11" s="95" customFormat="1">
       <c r="A206" s="325" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="B206" s="323">
         <v>713.64</v>
@@ -54072,7 +54065,7 @@
     </row>
     <row r="207" spans="1:11" s="95" customFormat="1">
       <c r="A207" s="325" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="B207" s="322"/>
       <c r="C207" s="322"/>
@@ -54091,7 +54084,7 @@
     </row>
     <row r="208" spans="1:11" s="95" customFormat="1">
       <c r="A208" s="334" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="B208" s="332">
         <v>2522.5</v>
@@ -54118,7 +54111,7 @@
     </row>
     <row r="209" spans="1:11" s="95" customFormat="1">
       <c r="A209" s="325" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="B209" s="322"/>
       <c r="C209" s="322"/>
@@ -54133,7 +54126,7 @@
     </row>
     <row r="210" spans="1:11" s="95" customFormat="1">
       <c r="A210" s="325" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="B210" s="321">
         <v>1467.55</v>
@@ -54177,7 +54170,7 @@
     </row>
     <row r="212" spans="1:11" s="95" customFormat="1">
       <c r="A212" s="325" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="B212" s="323">
         <v>23.22</v>
@@ -54196,7 +54189,7 @@
     </row>
     <row r="213" spans="1:11" s="95" customFormat="1">
       <c r="A213" s="325" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="B213" s="323">
         <v>6.42</v>
@@ -54215,7 +54208,7 @@
     </row>
     <row r="214" spans="1:11" s="95" customFormat="1">
       <c r="A214" s="325" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="B214" s="322"/>
       <c r="C214" s="322"/>
@@ -54234,7 +54227,7 @@
     </row>
     <row r="215" spans="1:11" s="95" customFormat="1">
       <c r="A215" s="334" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="B215" s="322"/>
       <c r="C215" s="322"/>
@@ -54257,7 +54250,7 @@
     </row>
     <row r="216" spans="1:11" s="95" customFormat="1">
       <c r="A216" s="325" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="B216" s="322"/>
       <c r="C216" s="322"/>
@@ -54278,7 +54271,7 @@
     </row>
     <row r="217" spans="1:11" s="95" customFormat="1">
       <c r="A217" s="322" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="B217" s="322"/>
       <c r="C217" s="322"/>
@@ -54297,7 +54290,7 @@
     </row>
     <row r="218" spans="1:11" s="95" customFormat="1">
       <c r="A218" s="334" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="B218" s="323">
         <v>694.14</v>
@@ -54316,7 +54309,7 @@
     </row>
     <row r="219" spans="1:11" s="95" customFormat="1">
       <c r="A219" s="325" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="B219" s="323">
         <v>672.91</v>
@@ -54335,7 +54328,7 @@
     </row>
     <row r="220" spans="1:11" s="95" customFormat="1">
       <c r="A220" s="325" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="B220" s="323">
         <v>21.23</v>
@@ -54354,7 +54347,7 @@
     </row>
     <row r="221" spans="1:11" s="95" customFormat="1">
       <c r="A221" s="327" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="B221" s="326"/>
       <c r="C221" s="326"/>
@@ -54396,7 +54389,7 @@
     </row>
     <row r="223" spans="1:11" s="95" customFormat="1">
       <c r="A223" s="325" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="B223" s="322"/>
       <c r="C223" s="322"/>
@@ -54417,7 +54410,7 @@
     </row>
     <row r="224" spans="1:11" s="95" customFormat="1">
       <c r="A224" s="325" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="B224" s="322"/>
       <c r="C224" s="322"/>
@@ -54438,7 +54431,7 @@
     </row>
     <row r="225" spans="1:11" s="95" customFormat="1">
       <c r="A225" s="325" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="B225" s="322"/>
       <c r="C225" s="322"/>
@@ -54457,7 +54450,7 @@
     </row>
     <row r="226" spans="1:11" s="95" customFormat="1">
       <c r="A226" s="325" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="B226" s="322"/>
       <c r="C226" s="322"/>
@@ -54478,7 +54471,7 @@
     </row>
     <row r="227" spans="1:11" s="95" customFormat="1">
       <c r="A227" s="327" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="B227" s="326"/>
       <c r="C227" s="328">
@@ -54562,7 +54555,7 @@
     </row>
     <row r="231" spans="1:11" s="95" customFormat="1">
       <c r="A231" s="325" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="B231" s="322"/>
       <c r="C231" s="323">
@@ -54581,7 +54574,7 @@
     </row>
     <row r="232" spans="1:11" s="95" customFormat="1">
       <c r="A232" s="325" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="B232" s="322"/>
       <c r="C232" s="322"/>
@@ -54598,7 +54591,7 @@
     </row>
     <row r="233" spans="1:11" s="95" customFormat="1">
       <c r="A233" s="325" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="B233" s="322"/>
       <c r="C233" s="322"/>
@@ -54615,7 +54608,7 @@
     </row>
     <row r="234" spans="1:11" s="95" customFormat="1">
       <c r="A234" s="325" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="B234" s="322"/>
       <c r="C234" s="322"/>
@@ -54632,7 +54625,7 @@
     </row>
     <row r="235" spans="1:11" s="95" customFormat="1">
       <c r="A235" s="327" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="B235" s="326"/>
       <c r="C235" s="326"/>
@@ -54653,7 +54646,7 @@
     </row>
     <row r="236" spans="1:11" s="95" customFormat="1">
       <c r="A236" s="325" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="B236" s="322"/>
       <c r="C236" s="322"/>
@@ -54672,7 +54665,7 @@
     </row>
     <row r="237" spans="1:11" s="95" customFormat="1">
       <c r="A237" s="325" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="B237" s="322"/>
       <c r="C237" s="322"/>
@@ -54691,7 +54684,7 @@
     </row>
     <row r="238" spans="1:11" s="95" customFormat="1">
       <c r="A238" s="325" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="B238" s="322"/>
       <c r="C238" s="322"/>
@@ -54712,7 +54705,7 @@
     </row>
     <row r="239" spans="1:11" s="95" customFormat="1">
       <c r="A239" s="325" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="B239" s="322"/>
       <c r="C239" s="322"/>
@@ -54731,7 +54724,7 @@
     </row>
     <row r="240" spans="1:11" s="95" customFormat="1">
       <c r="A240" s="325" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="B240" s="322"/>
       <c r="C240" s="322"/>
@@ -54752,7 +54745,7 @@
     </row>
     <row r="241" spans="1:11" s="95" customFormat="1">
       <c r="A241" s="327" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="B241" s="326"/>
       <c r="C241" s="326"/>
@@ -54813,7 +54806,7 @@
     </row>
     <row r="244" spans="1:11" s="95" customFormat="1">
       <c r="A244" s="325" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="B244" s="323">
         <v>273</v>
@@ -54836,7 +54829,7 @@
     </row>
     <row r="245" spans="1:11" s="95" customFormat="1">
       <c r="A245" s="322" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="B245" s="321">
         <v>376005</v>
@@ -54854,24 +54847,24 @@
       </c>
     </row>
     <row r="246" spans="1:11" s="95" customFormat="1" ht="15" customHeight="1">
-      <c r="A246" s="394" t="s">
-        <v>1726</v>
-      </c>
-      <c r="B246" s="395"/>
-      <c r="C246" s="395"/>
-      <c r="D246" s="395"/>
-      <c r="E246" s="395"/>
-      <c r="F246" s="395"/>
-      <c r="G246" s="395"/>
-      <c r="H246" s="395"/>
-      <c r="I246" s="395"/>
-      <c r="J246" s="395"/>
-      <c r="K246" s="396"/>
+      <c r="A246" s="395" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B246" s="396"/>
+      <c r="C246" s="396"/>
+      <c r="D246" s="396"/>
+      <c r="E246" s="396"/>
+      <c r="F246" s="396"/>
+      <c r="G246" s="396"/>
+      <c r="H246" s="396"/>
+      <c r="I246" s="396"/>
+      <c r="J246" s="396"/>
+      <c r="K246" s="397"/>
     </row>
     <row r="247" spans="1:11" s="95" customFormat="1"/>
     <row r="248" spans="1:11" s="95" customFormat="1" ht="28.5">
       <c r="A248" s="4" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="B248" s="320" t="s">
         <v>561</v>
@@ -54886,7 +54879,7 @@
     </row>
     <row r="249" spans="1:11" s="95" customFormat="1">
       <c r="A249" s="319" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="B249" s="318">
         <f>B154-C154</f>
@@ -54904,7 +54897,7 @@
     </row>
     <row r="250" spans="1:11" s="95" customFormat="1">
       <c r="A250" s="319" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="B250" s="318">
         <f>B249*$C$60</f>
@@ -54922,7 +54915,7 @@
     </row>
     <row r="251" spans="1:11" s="95" customFormat="1">
       <c r="A251" s="319" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="B251" s="318">
         <f>SUM(B250:E250)</f>
@@ -54936,24 +54929,24 @@
     <row r="253" spans="1:11" s="95" customFormat="1"/>
     <row r="254" spans="1:11" s="95" customFormat="1">
       <c r="A254" s="317" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="B254" s="84"/>
     </row>
     <row r="255" spans="1:11" s="95" customFormat="1">
       <c r="A255" s="95" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="256" spans="1:11" s="95" customFormat="1">
       <c r="A256" s="95" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
     </row>
     <row r="257" spans="1:4" s="95" customFormat="1"/>
     <row r="258" spans="1:4" s="95" customFormat="1">
       <c r="A258" s="95" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="B258" s="95">
         <v>719</v>
@@ -54961,7 +54954,7 @@
     </row>
     <row r="259" spans="1:4" s="95" customFormat="1">
       <c r="A259" s="95" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="B259" s="95">
         <v>11</v>
@@ -54969,7 +54962,7 @@
     </row>
     <row r="260" spans="1:4" s="95" customFormat="1">
       <c r="A260" s="95" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="B260" s="315">
         <f>B259/B258*10^6</f>
@@ -54980,86 +54973,86 @@
     <row r="262" spans="1:4" s="95" customFormat="1"/>
     <row r="263" spans="1:4" s="95" customFormat="1">
       <c r="A263" s="85" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="B263" s="84"/>
       <c r="C263" s="84"/>
     </row>
     <row r="264" spans="1:4" s="95" customFormat="1">
       <c r="A264" s="95" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="B264" s="315">
         <f>(B149-B251)/(2007-2000)*(2005-2000)+B251+B260</f>
         <v>1749351.5192827338</v>
       </c>
       <c r="C264" s="95" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="265" spans="1:4" s="95" customFormat="1">
       <c r="A265" s="95" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="B265" s="95">
         <f>B264/B266</f>
         <v>0.71977393159643066</v>
       </c>
       <c r="C265" s="95" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="266" spans="1:4" s="95" customFormat="1">
       <c r="A266" s="95" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="B266" s="95">
         <v>2430418</v>
       </c>
       <c r="C266" s="95" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="D266" s="95" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="267" spans="1:4" s="95" customFormat="1">
       <c r="A267" s="95" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="B267" s="95">
         <v>11162212</v>
       </c>
       <c r="C267" s="95" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="268" spans="1:4" s="95" customFormat="1">
       <c r="A268" s="95" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="B268" s="316">
         <v>0.33</v>
       </c>
       <c r="C268" s="95" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="269" spans="1:4" s="95" customFormat="1">
       <c r="A269" s="95" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="B269" s="316">
         <v>0.35</v>
       </c>
       <c r="C269" s="95" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="270" spans="1:4" s="95" customFormat="1"/>
     <row r="271" spans="1:4" s="95" customFormat="1">
       <c r="A271" s="95" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="B271" s="95">
         <f>B265*(1-B268)</f>
@@ -55068,7 +55061,7 @@
     </row>
     <row r="272" spans="1:4" s="95" customFormat="1">
       <c r="A272" s="95" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="B272" s="95">
         <f>B265*(1-B269)</f>
@@ -55078,51 +55071,51 @@
     <row r="273" spans="1:10" s="95" customFormat="1"/>
     <row r="274" spans="1:10" s="95" customFormat="1">
       <c r="A274" s="95" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="B274" s="95">
         <f>B267*B271</f>
         <v>5382960.3750904137</v>
       </c>
       <c r="C274" s="95" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="275" spans="1:10" s="95" customFormat="1">
       <c r="A275" s="95" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="B275" s="95">
         <f>B267*B272</f>
         <v>5222274.9907593569</v>
       </c>
       <c r="C275" s="95" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="276" spans="1:10" s="95" customFormat="1"/>
     <row r="277" spans="1:10" s="95" customFormat="1">
       <c r="A277" s="95" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="B277" s="315">
         <f>B274/1000</f>
         <v>5382.9603750904134</v>
       </c>
       <c r="C277" s="95" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="278" spans="1:10" s="95" customFormat="1">
       <c r="A278" s="95" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="B278" s="315">
         <f>B275/1000</f>
         <v>5222.274990759357</v>
       </c>
       <c r="C278" s="95" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="279" spans="1:10" s="23" customFormat="1">
@@ -64545,22 +64538,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="397" t="s">
+      <c r="A1" s="401" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="397"/>
-      <c r="C1" s="397"/>
-      <c r="D1" s="397"/>
-      <c r="E1" s="397"/>
+      <c r="B1" s="401"/>
+      <c r="C1" s="401"/>
+      <c r="D1" s="401"/>
+      <c r="E1" s="401"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="401" t="s">
+      <c r="A2" s="402" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="401"/>
-      <c r="C2" s="401"/>
-      <c r="D2" s="401"/>
-      <c r="E2" s="401"/>
+      <c r="B2" s="402"/>
+      <c r="C2" s="402"/>
+      <c r="D2" s="402"/>
+      <c r="E2" s="402"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="9" t="s">
@@ -64576,13 +64569,13 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="401" t="s">
+      <c r="A21" s="402" t="s">
         <v>173</v>
       </c>
-      <c r="B21" s="401"/>
-      <c r="C21" s="401"/>
-      <c r="D21" s="401"/>
-      <c r="E21" s="401"/>
+      <c r="B21" s="402"/>
+      <c r="C21" s="402"/>
+      <c r="D21" s="402"/>
+      <c r="E21" s="402"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="9" t="s">
@@ -64598,13 +64591,13 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="401" t="s">
+      <c r="A40" s="402" t="s">
         <v>174</v>
       </c>
-      <c r="B40" s="401"/>
-      <c r="C40" s="401"/>
-      <c r="D40" s="401"/>
-      <c r="E40" s="401"/>
+      <c r="B40" s="402"/>
+      <c r="C40" s="402"/>
+      <c r="D40" s="402"/>
+      <c r="E40" s="402"/>
     </row>
     <row r="57" spans="1:5" ht="14.65" thickBot="1">
       <c r="A57" s="9" t="s">
@@ -64620,13 +64613,13 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="397" t="s">
+      <c r="A60" s="401" t="s">
         <v>176</v>
       </c>
-      <c r="B60" s="397"/>
-      <c r="C60" s="397"/>
-      <c r="D60" s="397"/>
-      <c r="E60" s="397"/>
+      <c r="B60" s="401"/>
+      <c r="C60" s="401"/>
+      <c r="D60" s="401"/>
+      <c r="E60" s="401"/>
     </row>
     <row r="85" spans="1:39" s="12" customFormat="1">
       <c r="A85" s="9" t="s">
@@ -64731,13 +64724,13 @@
       </c>
     </row>
     <row r="89" spans="1:39">
-      <c r="A89" s="397" t="s">
+      <c r="A89" s="401" t="s">
         <v>177</v>
       </c>
-      <c r="B89" s="397"/>
-      <c r="C89" s="397"/>
-      <c r="D89" s="397"/>
-      <c r="E89" s="397"/>
+      <c r="B89" s="401"/>
+      <c r="C89" s="401"/>
+      <c r="D89" s="401"/>
+      <c r="E89" s="401"/>
     </row>
     <row r="90" spans="1:39">
       <c r="A90" s="9">
@@ -64824,13 +64817,13 @@
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="397" t="s">
+      <c r="A98" s="401" t="s">
         <v>178</v>
       </c>
-      <c r="B98" s="397"/>
-      <c r="C98" s="397"/>
-      <c r="D98" s="397"/>
-      <c r="E98" s="397"/>
+      <c r="B98" s="401"/>
+      <c r="C98" s="401"/>
+      <c r="D98" s="401"/>
+      <c r="E98" s="401"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="17">
@@ -64914,13 +64907,13 @@
       <c r="A108" s="20"/>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="397" t="s">
+      <c r="A109" s="401" t="s">
         <v>180</v>
       </c>
-      <c r="B109" s="397"/>
-      <c r="C109" s="397"/>
-      <c r="D109" s="397"/>
-      <c r="E109" s="397"/>
+      <c r="B109" s="401"/>
+      <c r="C109" s="401"/>
+      <c r="D109" s="401"/>
+      <c r="E109" s="401"/>
     </row>
     <row r="110" spans="1:5" ht="14.65" thickBot="1"/>
     <row r="111" spans="1:5" ht="14.65" thickBot="1">
@@ -64933,13 +64926,13 @@
       </c>
     </row>
     <row r="113" spans="1:14">
-      <c r="A113" s="397" t="s">
+      <c r="A113" s="401" t="s">
         <v>179</v>
       </c>
-      <c r="B113" s="397"/>
-      <c r="C113" s="397"/>
-      <c r="D113" s="397"/>
-      <c r="E113" s="397"/>
+      <c r="B113" s="401"/>
+      <c r="C113" s="401"/>
+      <c r="D113" s="401"/>
+      <c r="E113" s="401"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="17">
@@ -65020,13 +65013,13 @@
       </c>
     </row>
     <row r="124" spans="1:14">
-      <c r="A124" s="397" t="s">
+      <c r="A124" s="401" t="s">
         <v>435</v>
       </c>
-      <c r="B124" s="397"/>
-      <c r="C124" s="397"/>
-      <c r="D124" s="397"/>
-      <c r="E124" s="397"/>
+      <c r="B124" s="401"/>
+      <c r="C124" s="401"/>
+      <c r="D124" s="401"/>
+      <c r="E124" s="401"/>
       <c r="L124" s="21"/>
     </row>
     <row r="125" spans="1:14">
@@ -65117,13 +65110,13 @@
       <c r="C133" s="15"/>
     </row>
     <row r="134" spans="1:14">
-      <c r="A134" s="397" t="s">
+      <c r="A134" s="401" t="s">
         <v>110</v>
       </c>
-      <c r="B134" s="397"/>
-      <c r="C134" s="397"/>
-      <c r="D134" s="397"/>
-      <c r="E134" s="397"/>
+      <c r="B134" s="401"/>
+      <c r="C134" s="401"/>
+      <c r="D134" s="401"/>
+      <c r="E134" s="401"/>
     </row>
     <row r="135" spans="1:14">
       <c r="A135" s="27" t="s">
@@ -65703,13 +65696,13 @@
       <c r="G163" s="28"/>
     </row>
     <row r="165" spans="1:7">
-      <c r="A165" s="397" t="s">
+      <c r="A165" s="401" t="s">
         <v>183</v>
       </c>
-      <c r="B165" s="397"/>
-      <c r="C165" s="397"/>
-      <c r="D165" s="397"/>
-      <c r="E165" s="397"/>
+      <c r="B165" s="401"/>
+      <c r="C165" s="401"/>
+      <c r="D165" s="401"/>
+      <c r="E165" s="401"/>
     </row>
     <row r="166" spans="1:7" ht="14.65" thickBot="1">
       <c r="A166" s="23" t="s">
@@ -65732,10 +65725,10 @@
       <c r="B168" s="46"/>
     </row>
     <row r="169" spans="1:7">
-      <c r="A169" s="397" t="s">
+      <c r="A169" s="401" t="s">
         <v>443</v>
       </c>
-      <c r="B169" s="397"/>
+      <c r="B169" s="401"/>
     </row>
     <row r="170" spans="1:7">
       <c r="A170" s="23" t="s">
@@ -65767,13 +65760,13 @@
       <c r="B173" s="46"/>
     </row>
     <row r="174" spans="1:7">
-      <c r="A174" s="397" t="s">
+      <c r="A174" s="401" t="s">
         <v>192</v>
       </c>
-      <c r="B174" s="397"/>
-      <c r="C174" s="397"/>
-      <c r="D174" s="397"/>
-      <c r="E174" s="397"/>
+      <c r="B174" s="401"/>
+      <c r="C174" s="401"/>
+      <c r="D174" s="401"/>
+      <c r="E174" s="401"/>
     </row>
     <row r="175" spans="1:7" ht="14.65" thickBot="1">
       <c r="A175" s="23" t="s">
@@ -65793,13 +65786,13 @@
       </c>
     </row>
     <row r="178" spans="1:5">
-      <c r="A178" s="397" t="s">
+      <c r="A178" s="401" t="s">
         <v>186</v>
       </c>
-      <c r="B178" s="397"/>
-      <c r="C178" s="397"/>
-      <c r="D178" s="397"/>
-      <c r="E178" s="397"/>
+      <c r="B178" s="401"/>
+      <c r="C178" s="401"/>
+      <c r="D178" s="401"/>
+      <c r="E178" s="401"/>
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="25" t="s">
@@ -65827,13 +65820,13 @@
       </c>
     </row>
     <row r="183" spans="1:5">
-      <c r="A183" s="397" t="s">
+      <c r="A183" s="401" t="s">
         <v>188</v>
       </c>
-      <c r="B183" s="397"/>
-      <c r="C183" s="397"/>
-      <c r="D183" s="397"/>
-      <c r="E183" s="397"/>
+      <c r="B183" s="401"/>
+      <c r="C183" s="401"/>
+      <c r="D183" s="401"/>
+      <c r="E183" s="401"/>
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="23" t="s">
@@ -65888,13 +65881,13 @@
       </c>
     </row>
     <row r="191" spans="1:5">
-      <c r="A191" s="397" t="s">
+      <c r="A191" s="401" t="s">
         <v>202</v>
       </c>
-      <c r="B191" s="397"/>
-      <c r="C191" s="397"/>
-      <c r="D191" s="397"/>
-      <c r="E191" s="397"/>
+      <c r="B191" s="401"/>
+      <c r="C191" s="401"/>
+      <c r="D191" s="401"/>
+      <c r="E191" s="401"/>
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="21" t="s">
@@ -65954,6 +65947,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -65968,12 +65967,6 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Removed extraneous CO2 subscript in row 84 of the OutputGraphs tab
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -7427,9 +7427,6 @@
     <t>620e7a, c01b00, 004185, af64ff, 00b050, 04ffaf, 087bf1, c2dffd, 000000, f1bb18, f593e0, 969696</t>
   </si>
   <si>
-    <t>Output Transportation Sector Fuel Used by Vehicle Type[motorbikes,freight,CO2]; Output Transportation Sector Fuel Used by Vehicle Type[motorbikes,passenger,CO2]; Output Transportation Sector Fuel Used by Vehicle Type[ships,freight,CO2]; Output Transportation Sector Fuel Used by Vehicle Type[ships,passenger,CO2]; Output Transportation Sector Fuel Used by Vehicle Type[rail,freight,CO2]; Output Transportation Sector Fuel Used by Vehicle Type[rail,passenger,CO2]; Output Transportation Sector Fuel Used by Vehicle Type[aircraft,freight,CO2]; Output Transportation Sector Fuel Used by Vehicle Type[aircraft,passenger,CO2]; Output Transportation Sector Fuel Used by Vehicle Type[HDVs,freight,CO2]; Output Transportation Sector Fuel Used by Vehicle Type[HDVs,passenger,CO2]; Output Transportation Sector Fuel Used by Vehicle Type[LDVs,freight,CO2]; Output Transportation Sector Fuel Used by Vehicle Type[LDVs,passenger,CO2]</t>
-  </si>
-  <si>
     <t>620e7a, c01b00, 004185, af64ff, 00b050, 04ffaf, 087bf1, f1bb18, f593e0, c2dffd, 000000, 969696</t>
   </si>
   <si>
@@ -7487,6 +7484,9 @@
   </si>
   <si>
     <t>**Description:** This control setting adjusts the GDP impact of the recession caused by SARS-CoV-2 (COVID-19).  It is set in terms of the GDP growth rate for 2020, relative to 2019 (with negative values indicating GDP shrinkage).  Recession impacts can extend beyond 2020, and can be adjusted using the Implementation Schedule feature for this control setting.  // **Guidance for setting values:** As of 27 May 2020, projections for GDP impacts in India vary across several studies. Estimates by nine national and global agencies range between a GDP reduction of 2.3% on the optimistic end to a high of 11% (relative to an average counter-factual growth projection of 5.8%). On average, the projected reduction is 5.9%, resulting in a new GDP growth rate of -0.1%. This is the default setting.</t>
+  </si>
+  <si>
+    <t>Output Transportation Sector Fuel Used by Vehicle Type[motorbikes,freight]; Output Transportation Sector Fuel Used by Vehicle Type[motorbikes,passenger]; Output Transportation Sector Fuel Used by Vehicle Type[ships,freight]; Output Transportation Sector Fuel Used by Vehicle Type[ships,passenger]; Output Transportation Sector Fuel Used by Vehicle Type[rail,freight]; Output Transportation Sector Fuel Used by Vehicle Type[rail,passenger]; Output Transportation Sector Fuel Used by Vehicle Type[aircraft,freight]; Output Transportation Sector Fuel Used by Vehicle Type[aircraft,passenger]; Output Transportation Sector Fuel Used by Vehicle Type[HDVs,freight]; Output Transportation Sector Fuel Used by Vehicle Type[HDVs,passenger]; Output Transportation Sector Fuel Used by Vehicle Type[LDVs,freight]; Output Transportation Sector Fuel Used by Vehicle Type[LDVs,passenger]</t>
   </si>
 </sst>
 </file>
@@ -9603,6 +9603,9 @@
     <xf numFmtId="10" fontId="0" fillId="30" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -9629,9 +9632,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -10834,7 +10834,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="50" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="B16" s="176"/>
     </row>
@@ -10849,7 +10849,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="391" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="B18" s="118" t="str">
         <f t="array" ref="B18">IF(MIN(IF(COUNTIF(PolicyLevers!$H$2:$H$1500,PolicyLevers!$H$2:$H$1500)&gt;1,PolicyLevers!$H$2:$H$1500, ""))=0,"No duplicate ID numbers",MIN(IF(COUNTIF(PolicyLevers!$H$2:$H$1500,PolicyLevers!$H$2:$H$1500)&gt;1,PolicyLevers!$H$2:$H$1500, "")))</f>
@@ -10858,7 +10858,7 @@
     </row>
     <row r="19" spans="1:6" ht="28.5">
       <c r="A19" s="392" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="B19" s="118" t="str">
         <f>IF(MIN(IF((NOT(ISNUMBER(PolicyLevers!$H$2:$H$1500)))*(PolicyLevers!$I$2:$I$1500="Yes"),ROW(PolicyLevers!$H$2:$H$1500)))=0,"No missing ID numbers",MIN(IF((NOT(ISNUMBER(PolicyLevers!$H$2:$H$1500)))*(PolicyLevers!$I$2:$I$1500="Yes"),ROW(PolicyLevers!$H$2:$H$1500))))</f>
@@ -11014,8 +11014,8 @@
   <dimension ref="A1:T589"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A564" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P571" sqref="P571"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A84" sqref="A84:XFD84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -16810,7 +16810,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P96" s="177" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="Q96" s="76" t="str">
         <f t="shared" si="23"/>
@@ -21835,7 +21835,7 @@
         <v>39</v>
       </c>
       <c r="P178" s="180" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="Q178" s="55" t="s">
         <v>926</v>
@@ -36522,14 +36522,14 @@
         <v>967</v>
       </c>
       <c r="P436" s="183" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="Q436" s="10"/>
       <c r="R436" s="158" t="s">
         <v>1246</v>
       </c>
       <c r="S436" s="55" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="T436" s="10"/>
     </row>
@@ -44042,8 +44042,8 @@
       <c r="O571" s="4" t="s">
         <v>1434</v>
       </c>
-      <c r="P571" s="403" t="s">
-        <v>1963</v>
+      <c r="P571" s="394" t="s">
+        <v>1962</v>
       </c>
       <c r="R571" s="162"/>
       <c r="S571" s="67" t="s">
@@ -44521,10 +44521,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="394" t="s">
+      <c r="A1" s="395" t="s">
         <v>1415</v>
       </c>
-      <c r="B1" s="394"/>
+      <c r="B1" s="395"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="166" t="s">
@@ -44810,10 +44810,10 @@
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="394" t="s">
+      <c r="A37" s="395" t="s">
         <v>1419</v>
       </c>
-      <c r="B37" s="394"/>
+      <c r="B37" s="395"/>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="166" t="s">
@@ -44857,7 +44857,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G84" sqref="G84:I84"/>
+      <selection pane="bottomLeft" activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -47172,7 +47172,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="128.65" thickBot="1">
+    <row r="84" spans="1:9" ht="114.4" thickBot="1">
       <c r="A84" s="142" t="s">
         <v>791</v>
       </c>
@@ -47193,13 +47193,13 @@
         <v>petajoules / year</v>
       </c>
       <c r="G84" s="383" t="s">
-        <v>1950</v>
+        <v>1963</v>
       </c>
       <c r="H84" s="383" t="s">
         <v>1948</v>
       </c>
       <c r="I84" s="381" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="57">
@@ -50903,18 +50903,18 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="9" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>1959</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>1960</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="9" t="s">
+        <v>1960</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>1961</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>1962</v>
       </c>
     </row>
   </sheetData>
@@ -54847,19 +54847,19 @@
       </c>
     </row>
     <row r="246" spans="1:11" s="95" customFormat="1" ht="15" customHeight="1">
-      <c r="A246" s="395" t="s">
+      <c r="A246" s="396" t="s">
         <v>1725</v>
       </c>
-      <c r="B246" s="396"/>
-      <c r="C246" s="396"/>
-      <c r="D246" s="396"/>
-      <c r="E246" s="396"/>
-      <c r="F246" s="396"/>
-      <c r="G246" s="396"/>
-      <c r="H246" s="396"/>
-      <c r="I246" s="396"/>
-      <c r="J246" s="396"/>
-      <c r="K246" s="397"/>
+      <c r="B246" s="397"/>
+      <c r="C246" s="397"/>
+      <c r="D246" s="397"/>
+      <c r="E246" s="397"/>
+      <c r="F246" s="397"/>
+      <c r="G246" s="397"/>
+      <c r="H246" s="397"/>
+      <c r="I246" s="397"/>
+      <c r="J246" s="397"/>
+      <c r="K246" s="398"/>
     </row>
     <row r="247" spans="1:11" s="95" customFormat="1"/>
     <row r="248" spans="1:11" s="95" customFormat="1" ht="28.5">
@@ -64538,22 +64538,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="401" t="s">
+      <c r="A1" s="402" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="401"/>
-      <c r="C1" s="401"/>
-      <c r="D1" s="401"/>
-      <c r="E1" s="401"/>
+      <c r="B1" s="402"/>
+      <c r="C1" s="402"/>
+      <c r="D1" s="402"/>
+      <c r="E1" s="402"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="402" t="s">
+      <c r="A2" s="403" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="402"/>
-      <c r="C2" s="402"/>
-      <c r="D2" s="402"/>
-      <c r="E2" s="402"/>
+      <c r="B2" s="403"/>
+      <c r="C2" s="403"/>
+      <c r="D2" s="403"/>
+      <c r="E2" s="403"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="9" t="s">
@@ -64569,13 +64569,13 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="402" t="s">
+      <c r="A21" s="403" t="s">
         <v>173</v>
       </c>
-      <c r="B21" s="402"/>
-      <c r="C21" s="402"/>
-      <c r="D21" s="402"/>
-      <c r="E21" s="402"/>
+      <c r="B21" s="403"/>
+      <c r="C21" s="403"/>
+      <c r="D21" s="403"/>
+      <c r="E21" s="403"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="9" t="s">
@@ -64591,13 +64591,13 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="402" t="s">
+      <c r="A40" s="403" t="s">
         <v>174</v>
       </c>
-      <c r="B40" s="402"/>
-      <c r="C40" s="402"/>
-      <c r="D40" s="402"/>
-      <c r="E40" s="402"/>
+      <c r="B40" s="403"/>
+      <c r="C40" s="403"/>
+      <c r="D40" s="403"/>
+      <c r="E40" s="403"/>
     </row>
     <row r="57" spans="1:5" ht="14.65" thickBot="1">
       <c r="A57" s="9" t="s">
@@ -64613,13 +64613,13 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="401" t="s">
+      <c r="A60" s="402" t="s">
         <v>176</v>
       </c>
-      <c r="B60" s="401"/>
-      <c r="C60" s="401"/>
-      <c r="D60" s="401"/>
-      <c r="E60" s="401"/>
+      <c r="B60" s="402"/>
+      <c r="C60" s="402"/>
+      <c r="D60" s="402"/>
+      <c r="E60" s="402"/>
     </row>
     <row r="85" spans="1:39" s="12" customFormat="1">
       <c r="A85" s="9" t="s">
@@ -64724,13 +64724,13 @@
       </c>
     </row>
     <row r="89" spans="1:39">
-      <c r="A89" s="401" t="s">
+      <c r="A89" s="402" t="s">
         <v>177</v>
       </c>
-      <c r="B89" s="401"/>
-      <c r="C89" s="401"/>
-      <c r="D89" s="401"/>
-      <c r="E89" s="401"/>
+      <c r="B89" s="402"/>
+      <c r="C89" s="402"/>
+      <c r="D89" s="402"/>
+      <c r="E89" s="402"/>
     </row>
     <row r="90" spans="1:39">
       <c r="A90" s="9">
@@ -64817,13 +64817,13 @@
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="401" t="s">
+      <c r="A98" s="402" t="s">
         <v>178</v>
       </c>
-      <c r="B98" s="401"/>
-      <c r="C98" s="401"/>
-      <c r="D98" s="401"/>
-      <c r="E98" s="401"/>
+      <c r="B98" s="402"/>
+      <c r="C98" s="402"/>
+      <c r="D98" s="402"/>
+      <c r="E98" s="402"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="17">
@@ -64907,13 +64907,13 @@
       <c r="A108" s="20"/>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="401" t="s">
+      <c r="A109" s="402" t="s">
         <v>180</v>
       </c>
-      <c r="B109" s="401"/>
-      <c r="C109" s="401"/>
-      <c r="D109" s="401"/>
-      <c r="E109" s="401"/>
+      <c r="B109" s="402"/>
+      <c r="C109" s="402"/>
+      <c r="D109" s="402"/>
+      <c r="E109" s="402"/>
     </row>
     <row r="110" spans="1:5" ht="14.65" thickBot="1"/>
     <row r="111" spans="1:5" ht="14.65" thickBot="1">
@@ -64926,13 +64926,13 @@
       </c>
     </row>
     <row r="113" spans="1:14">
-      <c r="A113" s="401" t="s">
+      <c r="A113" s="402" t="s">
         <v>179</v>
       </c>
-      <c r="B113" s="401"/>
-      <c r="C113" s="401"/>
-      <c r="D113" s="401"/>
-      <c r="E113" s="401"/>
+      <c r="B113" s="402"/>
+      <c r="C113" s="402"/>
+      <c r="D113" s="402"/>
+      <c r="E113" s="402"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="17">
@@ -65013,13 +65013,13 @@
       </c>
     </row>
     <row r="124" spans="1:14">
-      <c r="A124" s="401" t="s">
+      <c r="A124" s="402" t="s">
         <v>435</v>
       </c>
-      <c r="B124" s="401"/>
-      <c r="C124" s="401"/>
-      <c r="D124" s="401"/>
-      <c r="E124" s="401"/>
+      <c r="B124" s="402"/>
+      <c r="C124" s="402"/>
+      <c r="D124" s="402"/>
+      <c r="E124" s="402"/>
       <c r="L124" s="21"/>
     </row>
     <row r="125" spans="1:14">
@@ -65110,13 +65110,13 @@
       <c r="C133" s="15"/>
     </row>
     <row r="134" spans="1:14">
-      <c r="A134" s="401" t="s">
+      <c r="A134" s="402" t="s">
         <v>110</v>
       </c>
-      <c r="B134" s="401"/>
-      <c r="C134" s="401"/>
-      <c r="D134" s="401"/>
-      <c r="E134" s="401"/>
+      <c r="B134" s="402"/>
+      <c r="C134" s="402"/>
+      <c r="D134" s="402"/>
+      <c r="E134" s="402"/>
     </row>
     <row r="135" spans="1:14">
       <c r="A135" s="27" t="s">
@@ -65131,25 +65131,25 @@
     </row>
     <row r="136" spans="1:14">
       <c r="A136" s="29"/>
-      <c r="B136" s="398" t="s">
+      <c r="B136" s="399" t="s">
         <v>452</v>
       </c>
-      <c r="C136" s="399"/>
-      <c r="D136" s="399"/>
-      <c r="E136" s="400"/>
+      <c r="C136" s="400"/>
+      <c r="D136" s="400"/>
+      <c r="E136" s="401"/>
       <c r="F136" s="28"/>
       <c r="G136" s="28"/>
     </row>
     <row r="137" spans="1:14">
       <c r="A137" s="30"/>
-      <c r="B137" s="398" t="s">
+      <c r="B137" s="399" t="s">
         <v>453</v>
       </c>
-      <c r="C137" s="400"/>
-      <c r="D137" s="398" t="s">
+      <c r="C137" s="401"/>
+      <c r="D137" s="399" t="s">
         <v>454</v>
       </c>
-      <c r="E137" s="400"/>
+      <c r="E137" s="401"/>
       <c r="F137" s="28"/>
       <c r="G137" s="28"/>
     </row>
@@ -65696,13 +65696,13 @@
       <c r="G163" s="28"/>
     </row>
     <row r="165" spans="1:7">
-      <c r="A165" s="401" t="s">
+      <c r="A165" s="402" t="s">
         <v>183</v>
       </c>
-      <c r="B165" s="401"/>
-      <c r="C165" s="401"/>
-      <c r="D165" s="401"/>
-      <c r="E165" s="401"/>
+      <c r="B165" s="402"/>
+      <c r="C165" s="402"/>
+      <c r="D165" s="402"/>
+      <c r="E165" s="402"/>
     </row>
     <row r="166" spans="1:7" ht="14.65" thickBot="1">
       <c r="A166" s="23" t="s">
@@ -65725,10 +65725,10 @@
       <c r="B168" s="46"/>
     </row>
     <row r="169" spans="1:7">
-      <c r="A169" s="401" t="s">
+      <c r="A169" s="402" t="s">
         <v>443</v>
       </c>
-      <c r="B169" s="401"/>
+      <c r="B169" s="402"/>
     </row>
     <row r="170" spans="1:7">
       <c r="A170" s="23" t="s">
@@ -65760,13 +65760,13 @@
       <c r="B173" s="46"/>
     </row>
     <row r="174" spans="1:7">
-      <c r="A174" s="401" t="s">
+      <c r="A174" s="402" t="s">
         <v>192</v>
       </c>
-      <c r="B174" s="401"/>
-      <c r="C174" s="401"/>
-      <c r="D174" s="401"/>
-      <c r="E174" s="401"/>
+      <c r="B174" s="402"/>
+      <c r="C174" s="402"/>
+      <c r="D174" s="402"/>
+      <c r="E174" s="402"/>
     </row>
     <row r="175" spans="1:7" ht="14.65" thickBot="1">
       <c r="A175" s="23" t="s">
@@ -65786,13 +65786,13 @@
       </c>
     </row>
     <row r="178" spans="1:5">
-      <c r="A178" s="401" t="s">
+      <c r="A178" s="402" t="s">
         <v>186</v>
       </c>
-      <c r="B178" s="401"/>
-      <c r="C178" s="401"/>
-      <c r="D178" s="401"/>
-      <c r="E178" s="401"/>
+      <c r="B178" s="402"/>
+      <c r="C178" s="402"/>
+      <c r="D178" s="402"/>
+      <c r="E178" s="402"/>
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="25" t="s">
@@ -65820,13 +65820,13 @@
       </c>
     </row>
     <row r="183" spans="1:5">
-      <c r="A183" s="401" t="s">
+      <c r="A183" s="402" t="s">
         <v>188</v>
       </c>
-      <c r="B183" s="401"/>
-      <c r="C183" s="401"/>
-      <c r="D183" s="401"/>
-      <c r="E183" s="401"/>
+      <c r="B183" s="402"/>
+      <c r="C183" s="402"/>
+      <c r="D183" s="402"/>
+      <c r="E183" s="402"/>
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="23" t="s">
@@ -65881,13 +65881,13 @@
       </c>
     </row>
     <row r="191" spans="1:5">
-      <c r="A191" s="401" t="s">
+      <c r="A191" s="402" t="s">
         <v>202</v>
       </c>
-      <c r="B191" s="401"/>
-      <c r="C191" s="401"/>
-      <c r="D191" s="401"/>
-      <c r="E191" s="401"/>
+      <c r="B191" s="402"/>
+      <c r="C191" s="402"/>
+      <c r="D191" s="402"/>
+      <c r="E191" s="402"/>
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="21" t="s">

</xml_diff>

<commit_message>
Corrected trailing semicolon in WebAppData and reference error in FoPITY files
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -7373,9 +7373,6 @@
     <t>620e7a, f1bb18, 00b050, c01b00, 000000</t>
   </si>
   <si>
-    <t>Output New Vehicles in Thousands[LDVs,freight,hydrogen vehicle]; Output New Vehicles in Thousands[LDVs,freight,battery electric vehicle]; Output New Vehicles in Thousands[LDVs,freight,plugin hybrid vehicle]; Output New Vehicles in Thousands[LDVs,freight,diesel vehicle];</t>
-  </si>
-  <si>
     <t>Hydrogen Vehicle, Battery Electric Vehicle, Plug-in Hybrid Vehicle, Diesel Engine Vehicle</t>
   </si>
   <si>
@@ -7487,6 +7484,9 @@
   </si>
   <si>
     <t>Output Transportation Sector Fuel Used by Vehicle Type[motorbikes,freight]; Output Transportation Sector Fuel Used by Vehicle Type[motorbikes,passenger]; Output Transportation Sector Fuel Used by Vehicle Type[ships,freight]; Output Transportation Sector Fuel Used by Vehicle Type[ships,passenger]; Output Transportation Sector Fuel Used by Vehicle Type[rail,freight]; Output Transportation Sector Fuel Used by Vehicle Type[rail,passenger]; Output Transportation Sector Fuel Used by Vehicle Type[aircraft,freight]; Output Transportation Sector Fuel Used by Vehicle Type[aircraft,passenger]; Output Transportation Sector Fuel Used by Vehicle Type[HDVs,freight]; Output Transportation Sector Fuel Used by Vehicle Type[HDVs,passenger]; Output Transportation Sector Fuel Used by Vehicle Type[LDVs,freight]; Output Transportation Sector Fuel Used by Vehicle Type[LDVs,passenger]</t>
+  </si>
+  <si>
+    <t>Output New Vehicles in Thousands[LDVs,freight,hydrogen vehicle]; Output New Vehicles in Thousands[LDVs,freight,battery electric vehicle]; Output New Vehicles in Thousands[LDVs,freight,plugin hybrid vehicle]; Output New Vehicles in Thousands[LDVs,freight,diesel vehicle]</t>
   </si>
 </sst>
 </file>
@@ -9618,6 +9618,9 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -9626,9 +9629,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -10834,7 +10834,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="50" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="B16" s="176"/>
     </row>
@@ -10849,7 +10849,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="391" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="B18" s="118" t="str">
         <f t="array" ref="B18">IF(MIN(IF(COUNTIF(PolicyLevers!$H$2:$H$1500,PolicyLevers!$H$2:$H$1500)&gt;1,PolicyLevers!$H$2:$H$1500, ""))=0,"No duplicate ID numbers",MIN(IF(COUNTIF(PolicyLevers!$H$2:$H$1500,PolicyLevers!$H$2:$H$1500)&gt;1,PolicyLevers!$H$2:$H$1500, "")))</f>
@@ -10858,7 +10858,7 @@
     </row>
     <row r="19" spans="1:6" ht="28.5">
       <c r="A19" s="392" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="B19" s="118" t="str">
         <f>IF(MIN(IF((NOT(ISNUMBER(PolicyLevers!$H$2:$H$1500)))*(PolicyLevers!$I$2:$I$1500="Yes"),ROW(PolicyLevers!$H$2:$H$1500)))=0,"No missing ID numbers",MIN(IF((NOT(ISNUMBER(PolicyLevers!$H$2:$H$1500)))*(PolicyLevers!$I$2:$I$1500="Yes"),ROW(PolicyLevers!$H$2:$H$1500))))</f>
@@ -11015,7 +11015,7 @@
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A84" sqref="A84:XFD84"/>
+      <selection pane="bottomLeft" activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -16810,7 +16810,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P96" s="177" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="Q96" s="76" t="str">
         <f t="shared" si="23"/>
@@ -21835,7 +21835,7 @@
         <v>39</v>
       </c>
       <c r="P178" s="180" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="Q178" s="55" t="s">
         <v>926</v>
@@ -36522,14 +36522,14 @@
         <v>967</v>
       </c>
       <c r="P436" s="183" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="Q436" s="10"/>
       <c r="R436" s="158" t="s">
         <v>1246</v>
       </c>
       <c r="S436" s="55" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="T436" s="10"/>
     </row>
@@ -44043,7 +44043,7 @@
         <v>1434</v>
       </c>
       <c r="P571" s="394" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="R571" s="162"/>
       <c r="S571" s="67" t="s">
@@ -44510,7 +44510,7 @@
   </sheetPr>
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
@@ -44855,9 +44855,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G85" sqref="G85"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -46835,13 +46835,13 @@
         <v>thousand vehicles / year</v>
       </c>
       <c r="G72" s="383" t="s">
+        <v>1963</v>
+      </c>
+      <c r="H72" s="383" t="s">
         <v>1932</v>
       </c>
-      <c r="H72" s="383" t="s">
+      <c r="I72" s="383" t="s">
         <v>1933</v>
-      </c>
-      <c r="I72" s="383" t="s">
-        <v>1934</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="42.75">
@@ -46865,13 +46865,13 @@
         <v>thousand vehicles / year</v>
       </c>
       <c r="G73" s="383" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="H73" s="383" t="s">
+        <v>1932</v>
+      </c>
+      <c r="I73" s="383" t="s">
         <v>1933</v>
-      </c>
-      <c r="I73" s="383" t="s">
-        <v>1934</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="28.5">
@@ -46879,7 +46879,7 @@
         <v>1313</v>
       </c>
       <c r="B74" s="384" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="C74" s="164">
         <v>1</v>
@@ -46909,7 +46909,7 @@
         <v>1313</v>
       </c>
       <c r="B75" s="384" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="C75" s="385">
         <v>1</v>
@@ -46924,13 +46924,13 @@
         <v>795</v>
       </c>
       <c r="G75" s="383" t="s">
+        <v>1937</v>
+      </c>
+      <c r="H75" s="383" t="s">
         <v>1938</v>
       </c>
-      <c r="H75" s="383" t="s">
+      <c r="I75" s="383" t="s">
         <v>1939</v>
-      </c>
-      <c r="I75" s="383" t="s">
-        <v>1940</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="57">
@@ -46984,7 +46984,7 @@
         <v>thousand vehicles</v>
       </c>
       <c r="G77" s="383" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="H77" s="383" t="s">
         <v>1930</v>
@@ -47014,13 +47014,13 @@
         <v>million vehicles</v>
       </c>
       <c r="G78" s="383" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="H78" s="383" t="s">
+        <v>1932</v>
+      </c>
+      <c r="I78" s="383" t="s">
         <v>1933</v>
-      </c>
-      <c r="I78" s="383" t="s">
-        <v>1934</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="42.75">
@@ -47044,13 +47044,13 @@
         <v>million vehicles</v>
       </c>
       <c r="G79" s="383" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="H79" s="383" t="s">
+        <v>1932</v>
+      </c>
+      <c r="I79" s="383" t="s">
         <v>1933</v>
-      </c>
-      <c r="I79" s="383" t="s">
-        <v>1934</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="28.9" thickBot="1">
@@ -47058,7 +47058,7 @@
         <v>1313</v>
       </c>
       <c r="B80" s="386" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="C80" s="171">
         <v>1</v>
@@ -47088,7 +47088,7 @@
         <v>1313</v>
       </c>
       <c r="B81" s="386" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="C81" s="387">
         <v>1</v>
@@ -47103,13 +47103,13 @@
         <v>794</v>
       </c>
       <c r="G81" s="383" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="H81" s="383" t="s">
+        <v>1938</v>
+      </c>
+      <c r="I81" s="383" t="s">
         <v>1939</v>
-      </c>
-      <c r="I81" s="383" t="s">
-        <v>1940</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="128.25">
@@ -47133,13 +47133,13 @@
         <v>million metric tons / year</v>
       </c>
       <c r="G82" s="383" t="s">
+        <v>1946</v>
+      </c>
+      <c r="H82" s="383" t="s">
         <v>1947</v>
       </c>
-      <c r="H82" s="383" t="s">
+      <c r="I82" s="383" t="s">
         <v>1948</v>
-      </c>
-      <c r="I82" s="383" t="s">
-        <v>1949</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="85.5">
@@ -47193,13 +47193,13 @@
         <v>petajoules / year</v>
       </c>
       <c r="G84" s="383" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="H84" s="383" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="I84" s="381" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="57">
@@ -50903,18 +50903,18 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="9" t="s">
+        <v>1957</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>1958</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>1959</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="9" t="s">
+        <v>1959</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>1960</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>1961</v>
       </c>
     </row>
   </sheetData>
@@ -64538,13 +64538,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="402" t="s">
+      <c r="A1" s="399" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="402"/>
-      <c r="C1" s="402"/>
-      <c r="D1" s="402"/>
-      <c r="E1" s="402"/>
+      <c r="B1" s="399"/>
+      <c r="C1" s="399"/>
+      <c r="D1" s="399"/>
+      <c r="E1" s="399"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="403" t="s">
@@ -64613,13 +64613,13 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="402" t="s">
+      <c r="A60" s="399" t="s">
         <v>176</v>
       </c>
-      <c r="B60" s="402"/>
-      <c r="C60" s="402"/>
-      <c r="D60" s="402"/>
-      <c r="E60" s="402"/>
+      <c r="B60" s="399"/>
+      <c r="C60" s="399"/>
+      <c r="D60" s="399"/>
+      <c r="E60" s="399"/>
     </row>
     <row r="85" spans="1:39" s="12" customFormat="1">
       <c r="A85" s="9" t="s">
@@ -64724,13 +64724,13 @@
       </c>
     </row>
     <row r="89" spans="1:39">
-      <c r="A89" s="402" t="s">
+      <c r="A89" s="399" t="s">
         <v>177</v>
       </c>
-      <c r="B89" s="402"/>
-      <c r="C89" s="402"/>
-      <c r="D89" s="402"/>
-      <c r="E89" s="402"/>
+      <c r="B89" s="399"/>
+      <c r="C89" s="399"/>
+      <c r="D89" s="399"/>
+      <c r="E89" s="399"/>
     </row>
     <row r="90" spans="1:39">
       <c r="A90" s="9">
@@ -64817,13 +64817,13 @@
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="402" t="s">
+      <c r="A98" s="399" t="s">
         <v>178</v>
       </c>
-      <c r="B98" s="402"/>
-      <c r="C98" s="402"/>
-      <c r="D98" s="402"/>
-      <c r="E98" s="402"/>
+      <c r="B98" s="399"/>
+      <c r="C98" s="399"/>
+      <c r="D98" s="399"/>
+      <c r="E98" s="399"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="17">
@@ -64907,13 +64907,13 @@
       <c r="A108" s="20"/>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="402" t="s">
+      <c r="A109" s="399" t="s">
         <v>180</v>
       </c>
-      <c r="B109" s="402"/>
-      <c r="C109" s="402"/>
-      <c r="D109" s="402"/>
-      <c r="E109" s="402"/>
+      <c r="B109" s="399"/>
+      <c r="C109" s="399"/>
+      <c r="D109" s="399"/>
+      <c r="E109" s="399"/>
     </row>
     <row r="110" spans="1:5" ht="14.65" thickBot="1"/>
     <row r="111" spans="1:5" ht="14.65" thickBot="1">
@@ -64926,13 +64926,13 @@
       </c>
     </row>
     <row r="113" spans="1:14">
-      <c r="A113" s="402" t="s">
+      <c r="A113" s="399" t="s">
         <v>179</v>
       </c>
-      <c r="B113" s="402"/>
-      <c r="C113" s="402"/>
-      <c r="D113" s="402"/>
-      <c r="E113" s="402"/>
+      <c r="B113" s="399"/>
+      <c r="C113" s="399"/>
+      <c r="D113" s="399"/>
+      <c r="E113" s="399"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="17">
@@ -65013,13 +65013,13 @@
       </c>
     </row>
     <row r="124" spans="1:14">
-      <c r="A124" s="402" t="s">
+      <c r="A124" s="399" t="s">
         <v>435</v>
       </c>
-      <c r="B124" s="402"/>
-      <c r="C124" s="402"/>
-      <c r="D124" s="402"/>
-      <c r="E124" s="402"/>
+      <c r="B124" s="399"/>
+      <c r="C124" s="399"/>
+      <c r="D124" s="399"/>
+      <c r="E124" s="399"/>
       <c r="L124" s="21"/>
     </row>
     <row r="125" spans="1:14">
@@ -65110,13 +65110,13 @@
       <c r="C133" s="15"/>
     </row>
     <row r="134" spans="1:14">
-      <c r="A134" s="402" t="s">
+      <c r="A134" s="399" t="s">
         <v>110</v>
       </c>
-      <c r="B134" s="402"/>
-      <c r="C134" s="402"/>
-      <c r="D134" s="402"/>
-      <c r="E134" s="402"/>
+      <c r="B134" s="399"/>
+      <c r="C134" s="399"/>
+      <c r="D134" s="399"/>
+      <c r="E134" s="399"/>
     </row>
     <row r="135" spans="1:14">
       <c r="A135" s="27" t="s">
@@ -65131,25 +65131,25 @@
     </row>
     <row r="136" spans="1:14">
       <c r="A136" s="29"/>
-      <c r="B136" s="399" t="s">
+      <c r="B136" s="400" t="s">
         <v>452</v>
       </c>
-      <c r="C136" s="400"/>
-      <c r="D136" s="400"/>
-      <c r="E136" s="401"/>
+      <c r="C136" s="401"/>
+      <c r="D136" s="401"/>
+      <c r="E136" s="402"/>
       <c r="F136" s="28"/>
       <c r="G136" s="28"/>
     </row>
     <row r="137" spans="1:14">
       <c r="A137" s="30"/>
-      <c r="B137" s="399" t="s">
+      <c r="B137" s="400" t="s">
         <v>453</v>
       </c>
-      <c r="C137" s="401"/>
-      <c r="D137" s="399" t="s">
+      <c r="C137" s="402"/>
+      <c r="D137" s="400" t="s">
         <v>454</v>
       </c>
-      <c r="E137" s="401"/>
+      <c r="E137" s="402"/>
       <c r="F137" s="28"/>
       <c r="G137" s="28"/>
     </row>
@@ -65696,13 +65696,13 @@
       <c r="G163" s="28"/>
     </row>
     <row r="165" spans="1:7">
-      <c r="A165" s="402" t="s">
+      <c r="A165" s="399" t="s">
         <v>183</v>
       </c>
-      <c r="B165" s="402"/>
-      <c r="C165" s="402"/>
-      <c r="D165" s="402"/>
-      <c r="E165" s="402"/>
+      <c r="B165" s="399"/>
+      <c r="C165" s="399"/>
+      <c r="D165" s="399"/>
+      <c r="E165" s="399"/>
     </row>
     <row r="166" spans="1:7" ht="14.65" thickBot="1">
       <c r="A166" s="23" t="s">
@@ -65725,10 +65725,10 @@
       <c r="B168" s="46"/>
     </row>
     <row r="169" spans="1:7">
-      <c r="A169" s="402" t="s">
+      <c r="A169" s="399" t="s">
         <v>443</v>
       </c>
-      <c r="B169" s="402"/>
+      <c r="B169" s="399"/>
     </row>
     <row r="170" spans="1:7">
       <c r="A170" s="23" t="s">
@@ -65760,13 +65760,13 @@
       <c r="B173" s="46"/>
     </row>
     <row r="174" spans="1:7">
-      <c r="A174" s="402" t="s">
+      <c r="A174" s="399" t="s">
         <v>192</v>
       </c>
-      <c r="B174" s="402"/>
-      <c r="C174" s="402"/>
-      <c r="D174" s="402"/>
-      <c r="E174" s="402"/>
+      <c r="B174" s="399"/>
+      <c r="C174" s="399"/>
+      <c r="D174" s="399"/>
+      <c r="E174" s="399"/>
     </row>
     <row r="175" spans="1:7" ht="14.65" thickBot="1">
       <c r="A175" s="23" t="s">
@@ -65786,13 +65786,13 @@
       </c>
     </row>
     <row r="178" spans="1:5">
-      <c r="A178" s="402" t="s">
+      <c r="A178" s="399" t="s">
         <v>186</v>
       </c>
-      <c r="B178" s="402"/>
-      <c r="C178" s="402"/>
-      <c r="D178" s="402"/>
-      <c r="E178" s="402"/>
+      <c r="B178" s="399"/>
+      <c r="C178" s="399"/>
+      <c r="D178" s="399"/>
+      <c r="E178" s="399"/>
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="25" t="s">
@@ -65820,13 +65820,13 @@
       </c>
     </row>
     <row r="183" spans="1:5">
-      <c r="A183" s="402" t="s">
+      <c r="A183" s="399" t="s">
         <v>188</v>
       </c>
-      <c r="B183" s="402"/>
-      <c r="C183" s="402"/>
-      <c r="D183" s="402"/>
-      <c r="E183" s="402"/>
+      <c r="B183" s="399"/>
+      <c r="C183" s="399"/>
+      <c r="D183" s="399"/>
+      <c r="E183" s="399"/>
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="23" t="s">
@@ -65881,13 +65881,13 @@
       </c>
     </row>
     <row r="191" spans="1:5">
-      <c r="A191" s="402" t="s">
+      <c r="A191" s="399" t="s">
         <v>202</v>
       </c>
-      <c r="B191" s="402"/>
-      <c r="C191" s="402"/>
-      <c r="D191" s="402"/>
-      <c r="E191" s="402"/>
+      <c r="B191" s="399"/>
+      <c r="C191" s="399"/>
+      <c r="D191" s="399"/>
+      <c r="E191" s="399"/>
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="21" t="s">
@@ -65947,12 +65947,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -65967,6 +65961,12 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Remove TDM from WebAppData
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PolicyLevers!$A$1:$T$571</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -9600,6 +9600,9 @@
     <xf numFmtId="10" fontId="0" fillId="30" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -9612,6 +9615,9 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -9621,14 +9627,8 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -11010,9 +11010,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T589"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P90" sqref="P90"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I116" sqref="I116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -14733,7 +14733,7 @@
       <c r="O62" s="3" t="s">
         <v>937</v>
       </c>
-      <c r="P62" s="402" t="s">
+      <c r="P62" s="393" t="s">
         <v>1962</v>
       </c>
       <c r="R62" s="153" t="s">
@@ -17961,7 +17961,7 @@
         <v>179</v>
       </c>
       <c r="I115" s="55" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J115" s="76" t="str">
         <f t="shared" ref="J115:S115" si="35">J$114</f>
@@ -44518,10 +44518,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="393" t="s">
+      <c r="A1" s="394" t="s">
         <v>1415</v>
       </c>
-      <c r="B1" s="393"/>
+      <c r="B1" s="394"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="166" t="s">
@@ -44807,10 +44807,10 @@
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="393" t="s">
+      <c r="A37" s="394" t="s">
         <v>1419</v>
       </c>
-      <c r="B37" s="393"/>
+      <c r="B37" s="394"/>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="166" t="s">
@@ -54844,19 +54844,19 @@
       </c>
     </row>
     <row r="246" spans="1:11" s="95" customFormat="1" ht="15" customHeight="1">
-      <c r="A246" s="394" t="s">
+      <c r="A246" s="395" t="s">
         <v>1723</v>
       </c>
-      <c r="B246" s="395"/>
-      <c r="C246" s="395"/>
-      <c r="D246" s="395"/>
-      <c r="E246" s="395"/>
-      <c r="F246" s="395"/>
-      <c r="G246" s="395"/>
-      <c r="H246" s="395"/>
-      <c r="I246" s="395"/>
-      <c r="J246" s="395"/>
-      <c r="K246" s="396"/>
+      <c r="B246" s="396"/>
+      <c r="C246" s="396"/>
+      <c r="D246" s="396"/>
+      <c r="E246" s="396"/>
+      <c r="F246" s="396"/>
+      <c r="G246" s="396"/>
+      <c r="H246" s="396"/>
+      <c r="I246" s="396"/>
+      <c r="J246" s="396"/>
+      <c r="K246" s="397"/>
     </row>
     <row r="247" spans="1:11" s="95" customFormat="1"/>
     <row r="248" spans="1:11" s="95" customFormat="1" ht="28.5">
@@ -64535,22 +64535,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="400" t="s">
+      <c r="A1" s="398" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="400"/>
-      <c r="C1" s="400"/>
-      <c r="D1" s="400"/>
-      <c r="E1" s="400"/>
+      <c r="B1" s="398"/>
+      <c r="C1" s="398"/>
+      <c r="D1" s="398"/>
+      <c r="E1" s="398"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="401" t="s">
+      <c r="A2" s="402" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="401"/>
-      <c r="C2" s="401"/>
-      <c r="D2" s="401"/>
-      <c r="E2" s="401"/>
+      <c r="B2" s="402"/>
+      <c r="C2" s="402"/>
+      <c r="D2" s="402"/>
+      <c r="E2" s="402"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="9" t="s">
@@ -64566,13 +64566,13 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="401" t="s">
+      <c r="A21" s="402" t="s">
         <v>173</v>
       </c>
-      <c r="B21" s="401"/>
-      <c r="C21" s="401"/>
-      <c r="D21" s="401"/>
-      <c r="E21" s="401"/>
+      <c r="B21" s="402"/>
+      <c r="C21" s="402"/>
+      <c r="D21" s="402"/>
+      <c r="E21" s="402"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="9" t="s">
@@ -64588,13 +64588,13 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="401" t="s">
+      <c r="A40" s="402" t="s">
         <v>174</v>
       </c>
-      <c r="B40" s="401"/>
-      <c r="C40" s="401"/>
-      <c r="D40" s="401"/>
-      <c r="E40" s="401"/>
+      <c r="B40" s="402"/>
+      <c r="C40" s="402"/>
+      <c r="D40" s="402"/>
+      <c r="E40" s="402"/>
     </row>
     <row r="57" spans="1:5" ht="14.65" thickBot="1">
       <c r="A57" s="9" t="s">
@@ -64610,13 +64610,13 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="400" t="s">
+      <c r="A60" s="398" t="s">
         <v>176</v>
       </c>
-      <c r="B60" s="400"/>
-      <c r="C60" s="400"/>
-      <c r="D60" s="400"/>
-      <c r="E60" s="400"/>
+      <c r="B60" s="398"/>
+      <c r="C60" s="398"/>
+      <c r="D60" s="398"/>
+      <c r="E60" s="398"/>
     </row>
     <row r="85" spans="1:39" s="12" customFormat="1">
       <c r="A85" s="9" t="s">
@@ -64721,13 +64721,13 @@
       </c>
     </row>
     <row r="89" spans="1:39">
-      <c r="A89" s="400" t="s">
+      <c r="A89" s="398" t="s">
         <v>177</v>
       </c>
-      <c r="B89" s="400"/>
-      <c r="C89" s="400"/>
-      <c r="D89" s="400"/>
-      <c r="E89" s="400"/>
+      <c r="B89" s="398"/>
+      <c r="C89" s="398"/>
+      <c r="D89" s="398"/>
+      <c r="E89" s="398"/>
     </row>
     <row r="90" spans="1:39">
       <c r="A90" s="9">
@@ -64814,13 +64814,13 @@
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="400" t="s">
+      <c r="A98" s="398" t="s">
         <v>178</v>
       </c>
-      <c r="B98" s="400"/>
-      <c r="C98" s="400"/>
-      <c r="D98" s="400"/>
-      <c r="E98" s="400"/>
+      <c r="B98" s="398"/>
+      <c r="C98" s="398"/>
+      <c r="D98" s="398"/>
+      <c r="E98" s="398"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="17">
@@ -64904,13 +64904,13 @@
       <c r="A108" s="20"/>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="400" t="s">
+      <c r="A109" s="398" t="s">
         <v>180</v>
       </c>
-      <c r="B109" s="400"/>
-      <c r="C109" s="400"/>
-      <c r="D109" s="400"/>
-      <c r="E109" s="400"/>
+      <c r="B109" s="398"/>
+      <c r="C109" s="398"/>
+      <c r="D109" s="398"/>
+      <c r="E109" s="398"/>
     </row>
     <row r="110" spans="1:5" ht="14.65" thickBot="1"/>
     <row r="111" spans="1:5" ht="14.65" thickBot="1">
@@ -64923,13 +64923,13 @@
       </c>
     </row>
     <row r="113" spans="1:14">
-      <c r="A113" s="400" t="s">
+      <c r="A113" s="398" t="s">
         <v>179</v>
       </c>
-      <c r="B113" s="400"/>
-      <c r="C113" s="400"/>
-      <c r="D113" s="400"/>
-      <c r="E113" s="400"/>
+      <c r="B113" s="398"/>
+      <c r="C113" s="398"/>
+      <c r="D113" s="398"/>
+      <c r="E113" s="398"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="17">
@@ -65010,13 +65010,13 @@
       </c>
     </row>
     <row r="124" spans="1:14">
-      <c r="A124" s="400" t="s">
+      <c r="A124" s="398" t="s">
         <v>435</v>
       </c>
-      <c r="B124" s="400"/>
-      <c r="C124" s="400"/>
-      <c r="D124" s="400"/>
-      <c r="E124" s="400"/>
+      <c r="B124" s="398"/>
+      <c r="C124" s="398"/>
+      <c r="D124" s="398"/>
+      <c r="E124" s="398"/>
       <c r="L124" s="21"/>
     </row>
     <row r="125" spans="1:14">
@@ -65107,13 +65107,13 @@
       <c r="C133" s="15"/>
     </row>
     <row r="134" spans="1:14">
-      <c r="A134" s="400" t="s">
+      <c r="A134" s="398" t="s">
         <v>110</v>
       </c>
-      <c r="B134" s="400"/>
-      <c r="C134" s="400"/>
-      <c r="D134" s="400"/>
-      <c r="E134" s="400"/>
+      <c r="B134" s="398"/>
+      <c r="C134" s="398"/>
+      <c r="D134" s="398"/>
+      <c r="E134" s="398"/>
     </row>
     <row r="135" spans="1:14">
       <c r="A135" s="27" t="s">
@@ -65128,25 +65128,25 @@
     </row>
     <row r="136" spans="1:14">
       <c r="A136" s="29"/>
-      <c r="B136" s="397" t="s">
+      <c r="B136" s="399" t="s">
         <v>452</v>
       </c>
-      <c r="C136" s="398"/>
-      <c r="D136" s="398"/>
-      <c r="E136" s="399"/>
+      <c r="C136" s="400"/>
+      <c r="D136" s="400"/>
+      <c r="E136" s="401"/>
       <c r="F136" s="28"/>
       <c r="G136" s="28"/>
     </row>
     <row r="137" spans="1:14">
       <c r="A137" s="30"/>
-      <c r="B137" s="397" t="s">
+      <c r="B137" s="399" t="s">
         <v>453</v>
       </c>
-      <c r="C137" s="399"/>
-      <c r="D137" s="397" t="s">
+      <c r="C137" s="401"/>
+      <c r="D137" s="399" t="s">
         <v>454</v>
       </c>
-      <c r="E137" s="399"/>
+      <c r="E137" s="401"/>
       <c r="F137" s="28"/>
       <c r="G137" s="28"/>
     </row>
@@ -65693,13 +65693,13 @@
       <c r="G163" s="28"/>
     </row>
     <row r="165" spans="1:7">
-      <c r="A165" s="400" t="s">
+      <c r="A165" s="398" t="s">
         <v>183</v>
       </c>
-      <c r="B165" s="400"/>
-      <c r="C165" s="400"/>
-      <c r="D165" s="400"/>
-      <c r="E165" s="400"/>
+      <c r="B165" s="398"/>
+      <c r="C165" s="398"/>
+      <c r="D165" s="398"/>
+      <c r="E165" s="398"/>
     </row>
     <row r="166" spans="1:7" ht="14.65" thickBot="1">
       <c r="A166" s="23" t="s">
@@ -65722,10 +65722,10 @@
       <c r="B168" s="46"/>
     </row>
     <row r="169" spans="1:7">
-      <c r="A169" s="400" t="s">
+      <c r="A169" s="398" t="s">
         <v>443</v>
       </c>
-      <c r="B169" s="400"/>
+      <c r="B169" s="398"/>
     </row>
     <row r="170" spans="1:7">
       <c r="A170" s="23" t="s">
@@ -65757,13 +65757,13 @@
       <c r="B173" s="46"/>
     </row>
     <row r="174" spans="1:7">
-      <c r="A174" s="400" t="s">
+      <c r="A174" s="398" t="s">
         <v>192</v>
       </c>
-      <c r="B174" s="400"/>
-      <c r="C174" s="400"/>
-      <c r="D174" s="400"/>
-      <c r="E174" s="400"/>
+      <c r="B174" s="398"/>
+      <c r="C174" s="398"/>
+      <c r="D174" s="398"/>
+      <c r="E174" s="398"/>
     </row>
     <row r="175" spans="1:7" ht="14.65" thickBot="1">
       <c r="A175" s="23" t="s">
@@ -65783,13 +65783,13 @@
       </c>
     </row>
     <row r="178" spans="1:5">
-      <c r="A178" s="400" t="s">
+      <c r="A178" s="398" t="s">
         <v>186</v>
       </c>
-      <c r="B178" s="400"/>
-      <c r="C178" s="400"/>
-      <c r="D178" s="400"/>
-      <c r="E178" s="400"/>
+      <c r="B178" s="398"/>
+      <c r="C178" s="398"/>
+      <c r="D178" s="398"/>
+      <c r="E178" s="398"/>
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="25" t="s">
@@ -65817,13 +65817,13 @@
       </c>
     </row>
     <row r="183" spans="1:5">
-      <c r="A183" s="400" t="s">
+      <c r="A183" s="398" t="s">
         <v>188</v>
       </c>
-      <c r="B183" s="400"/>
-      <c r="C183" s="400"/>
-      <c r="D183" s="400"/>
-      <c r="E183" s="400"/>
+      <c r="B183" s="398"/>
+      <c r="C183" s="398"/>
+      <c r="D183" s="398"/>
+      <c r="E183" s="398"/>
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="23" t="s">
@@ -65878,13 +65878,13 @@
       </c>
     </row>
     <row r="191" spans="1:5">
-      <c r="A191" s="400" t="s">
+      <c r="A191" s="398" t="s">
         <v>202</v>
       </c>
-      <c r="B191" s="400"/>
-      <c r="C191" s="400"/>
-      <c r="D191" s="400"/>
-      <c r="E191" s="400"/>
+      <c r="B191" s="398"/>
+      <c r="C191" s="398"/>
+      <c r="D191" s="398"/>
+      <c r="E191" s="398"/>
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="21" t="s">
@@ -65944,12 +65944,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -65964,6 +65958,12 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Edit to CES guidance text (no data changes)
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PolicyLevers!$A$1:$T$571</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
 </workbook>
 </file>
 
@@ -7421,9 +7421,6 @@
     <t>620e7a, c01b00, 004185, af64ff, 00b050, 04ffaf, 087bf1, f1bb18, f593e0, c2dffd, 000000, 969696</t>
   </si>
   <si>
-    <t>**Description:** This policy specifies an increase in the fraction of electricity generation that must come from qualifying carbon-free sources (wind, solar, biomass, nuclear, hydro, and geothermal) in 2050.  This policy has no effect until the user-set value exceeds the existing fraction of carbon-free electricity and any carbon-free electricity standards which have been enacted at the state level. // **Guidance for setting values:** India's Ministry of Power has recently notified the growth trajectory of solar- and non-solar Renewable Purchase Obligations (RPOs) for all states to reach a total RPO target of 21% by 2022, which is held constant thereafter till 2050 in the BAU case.</t>
-  </si>
-  <si>
     <t>**Description:** This policy causes a percentage of merchant hydrogen (i.e. hydrogen produced for sale, not hydrogen produced and consumed on-site within a facility) to be produced via electrolysis rather than via other production pathways. // **Guidance for setting values:** Hydrogen production using electrolysis in India is in the R&amp;D stage. Oil and Natural Gas Corporation Energy Centre (OEC) has implemented a few research projects on the electrolysis of Copper-Chlorine for hydrogen production. There is no hydrogen production in the BAU case.</t>
   </si>
   <si>
@@ -7487,6 +7484,10 @@
   </si>
   <si>
     <t>**Description:** This policy specifies a percentage improvement in fuel economy (distance traveled on the same quantity of fuel with the same cargo or passenger loading) due to fuel economy standards for new light-duty freight vehicles (light commercial trucks) with gasoline or diesel engines. // **Guidance for setting values:** India has recently notified testing standards for Light and Medium Commercial freight vehicles with Gross Vehicle Weight (GVW) of 3.5 - 12 tonnes. To be implemented from April 2020, the fuel economy testing standards range between 14 km/liter to 5 km/liter for GVW of 3.5 tonnes and 12 tonnes respectively. In the current BAU case, new freight LDV fuel economy is not projected to change, and is constant at 20 km/liter between 2018-2050.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description:** This policy specifies an increase in the fraction of electricity generation that must come from qualifying carbon-free sources (wind, solar, geothermal, and municipal solid waste) in 2050.  This policy has no effect until the user-set value exceeds the existing fraction of carbon-free electricity and any carbon-free electricity standards which have been enacted at the state level. // **Guidance for setting values:** India's Renewable Purchase Obligations (RPOs) in the BAU case are differentiated by solar and non-solar (excluding hydro). The Ministry of Power has recently notified the growth trajectory of solar- and non-solar RPOs for all states to reach a total RPO target of 21% by 2022, which is held constant thereafter till 2050 in the BAU case. Non-solar BAU RPOs include wind and biomass. 
+In the non-BAU case, the lever setting is a total RPO target that includes generation from wind, solar, geothermal, and Municipal Solid Waste (MSW) sources. Geothermal and MSW are included as they may be feasible for a more ambitious Renewable Energy (RE) scenario with a delayed start. Biomass is excluded because it has issues such as adverse impacts on local air quality, competing land use, and feedstock availability challenges. Nuclear is excluded because of the need to manage radioactive waste, and large-hydro is not included due to potential state-level challenges in implementing additional capacity. When setting a high target with this lever, users should also turn on supporting power sector policies (i.e., Grid-Scale Electricity Storage, Increase Transmission, and Demand Response) to avoid curtailment of renewables. </t>
   </si>
 </sst>
 </file>
@@ -9615,9 +9616,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -9626,6 +9624,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -10831,7 +10832,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="50" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="B16" s="176"/>
     </row>
@@ -10846,7 +10847,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="390" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="B18" s="118" t="str">
         <f t="array" ref="B18">IF(MIN(IF(COUNTIF(PolicyLevers!$H$2:$H$1500,PolicyLevers!$H$2:$H$1500)&gt;1,PolicyLevers!$H$2:$H$1500, ""))=0,"No duplicate ID numbers",MIN(IF(COUNTIF(PolicyLevers!$H$2:$H$1500,PolicyLevers!$H$2:$H$1500)&gt;1,PolicyLevers!$H$2:$H$1500, "")))</f>
@@ -10855,7 +10856,7 @@
     </row>
     <row r="19" spans="1:6" ht="28.5">
       <c r="A19" s="391" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="B19" s="118" t="str">
         <f>IF(MIN(IF((NOT(ISNUMBER(PolicyLevers!$H$2:$H$1500)))*(PolicyLevers!$I$2:$I$1500="Yes"),ROW(PolicyLevers!$H$2:$H$1500)))=0,"No missing ID numbers",MIN(IF((NOT(ISNUMBER(PolicyLevers!$H$2:$H$1500)))*(PolicyLevers!$I$2:$I$1500="Yes"),ROW(PolicyLevers!$H$2:$H$1500))))</f>
@@ -11011,8 +11012,8 @@
   <dimension ref="A1:T589"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I116" sqref="I116"/>
+      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P178" sqref="P178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -14734,7 +14735,7 @@
         <v>937</v>
       </c>
       <c r="P62" s="393" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="R62" s="153" t="s">
         <v>1237</v>
@@ -16371,7 +16372,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P90" s="177" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="Q90" s="76" t="str">
         <f t="shared" si="23"/>
@@ -16807,7 +16808,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P96" s="177" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="Q96" s="76" t="str">
         <f t="shared" si="23"/>
@@ -21793,7 +21794,7 @@
       <c r="S177" s="57"/>
       <c r="T177" s="57"/>
     </row>
-    <row r="178" spans="1:20" s="5" customFormat="1" ht="99.75">
+    <row r="178" spans="1:20" s="5" customFormat="1" ht="185.25">
       <c r="A178" s="96" t="s">
         <v>8</v>
       </c>
@@ -21831,8 +21832,8 @@
       <c r="O178" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="P178" s="179" t="s">
-        <v>1948</v>
+      <c r="P178" s="183" t="s">
+        <v>1963</v>
       </c>
       <c r="Q178" s="55" t="s">
         <v>926</v>
@@ -36519,14 +36520,14 @@
         <v>967</v>
       </c>
       <c r="P436" s="182" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="Q436" s="10"/>
       <c r="R436" s="158" t="s">
         <v>1246</v>
       </c>
       <c r="S436" s="55" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="T436" s="10"/>
     </row>
@@ -44040,7 +44041,7 @@
         <v>1434</v>
       </c>
       <c r="P571" s="4" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="R571" s="162"/>
       <c r="S571" s="67" t="s">
@@ -46832,7 +46833,7 @@
         <v>thousand vehicles / year</v>
       </c>
       <c r="G72" s="382" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="H72" s="382" t="s">
         <v>1930</v>
@@ -47190,7 +47191,7 @@
         <v>petajoules / year</v>
       </c>
       <c r="G84" s="382" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="H84" s="382" t="s">
         <v>1945</v>
@@ -50900,18 +50901,18 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="9" t="s">
+        <v>1954</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>1955</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>1956</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="9" t="s">
+        <v>1956</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>1957</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>1958</v>
       </c>
     </row>
   </sheetData>
@@ -64535,13 +64536,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="398" t="s">
+      <c r="A1" s="401" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="398"/>
-      <c r="C1" s="398"/>
-      <c r="D1" s="398"/>
-      <c r="E1" s="398"/>
+      <c r="B1" s="401"/>
+      <c r="C1" s="401"/>
+      <c r="D1" s="401"/>
+      <c r="E1" s="401"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="402" t="s">
@@ -64610,13 +64611,13 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="398" t="s">
+      <c r="A60" s="401" t="s">
         <v>176</v>
       </c>
-      <c r="B60" s="398"/>
-      <c r="C60" s="398"/>
-      <c r="D60" s="398"/>
-      <c r="E60" s="398"/>
+      <c r="B60" s="401"/>
+      <c r="C60" s="401"/>
+      <c r="D60" s="401"/>
+      <c r="E60" s="401"/>
     </row>
     <row r="85" spans="1:39" s="12" customFormat="1">
       <c r="A85" s="9" t="s">
@@ -64721,13 +64722,13 @@
       </c>
     </row>
     <row r="89" spans="1:39">
-      <c r="A89" s="398" t="s">
+      <c r="A89" s="401" t="s">
         <v>177</v>
       </c>
-      <c r="B89" s="398"/>
-      <c r="C89" s="398"/>
-      <c r="D89" s="398"/>
-      <c r="E89" s="398"/>
+      <c r="B89" s="401"/>
+      <c r="C89" s="401"/>
+      <c r="D89" s="401"/>
+      <c r="E89" s="401"/>
     </row>
     <row r="90" spans="1:39">
       <c r="A90" s="9">
@@ -64814,13 +64815,13 @@
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="398" t="s">
+      <c r="A98" s="401" t="s">
         <v>178</v>
       </c>
-      <c r="B98" s="398"/>
-      <c r="C98" s="398"/>
-      <c r="D98" s="398"/>
-      <c r="E98" s="398"/>
+      <c r="B98" s="401"/>
+      <c r="C98" s="401"/>
+      <c r="D98" s="401"/>
+      <c r="E98" s="401"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="17">
@@ -64904,13 +64905,13 @@
       <c r="A108" s="20"/>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="398" t="s">
+      <c r="A109" s="401" t="s">
         <v>180</v>
       </c>
-      <c r="B109" s="398"/>
-      <c r="C109" s="398"/>
-      <c r="D109" s="398"/>
-      <c r="E109" s="398"/>
+      <c r="B109" s="401"/>
+      <c r="C109" s="401"/>
+      <c r="D109" s="401"/>
+      <c r="E109" s="401"/>
     </row>
     <row r="110" spans="1:5" ht="14.65" thickBot="1"/>
     <row r="111" spans="1:5" ht="14.65" thickBot="1">
@@ -64923,13 +64924,13 @@
       </c>
     </row>
     <row r="113" spans="1:14">
-      <c r="A113" s="398" t="s">
+      <c r="A113" s="401" t="s">
         <v>179</v>
       </c>
-      <c r="B113" s="398"/>
-      <c r="C113" s="398"/>
-      <c r="D113" s="398"/>
-      <c r="E113" s="398"/>
+      <c r="B113" s="401"/>
+      <c r="C113" s="401"/>
+      <c r="D113" s="401"/>
+      <c r="E113" s="401"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="17">
@@ -65010,13 +65011,13 @@
       </c>
     </row>
     <row r="124" spans="1:14">
-      <c r="A124" s="398" t="s">
+      <c r="A124" s="401" t="s">
         <v>435</v>
       </c>
-      <c r="B124" s="398"/>
-      <c r="C124" s="398"/>
-      <c r="D124" s="398"/>
-      <c r="E124" s="398"/>
+      <c r="B124" s="401"/>
+      <c r="C124" s="401"/>
+      <c r="D124" s="401"/>
+      <c r="E124" s="401"/>
       <c r="L124" s="21"/>
     </row>
     <row r="125" spans="1:14">
@@ -65107,13 +65108,13 @@
       <c r="C133" s="15"/>
     </row>
     <row r="134" spans="1:14">
-      <c r="A134" s="398" t="s">
+      <c r="A134" s="401" t="s">
         <v>110</v>
       </c>
-      <c r="B134" s="398"/>
-      <c r="C134" s="398"/>
-      <c r="D134" s="398"/>
-      <c r="E134" s="398"/>
+      <c r="B134" s="401"/>
+      <c r="C134" s="401"/>
+      <c r="D134" s="401"/>
+      <c r="E134" s="401"/>
     </row>
     <row r="135" spans="1:14">
       <c r="A135" s="27" t="s">
@@ -65128,25 +65129,25 @@
     </row>
     <row r="136" spans="1:14">
       <c r="A136" s="29"/>
-      <c r="B136" s="399" t="s">
+      <c r="B136" s="398" t="s">
         <v>452</v>
       </c>
-      <c r="C136" s="400"/>
-      <c r="D136" s="400"/>
-      <c r="E136" s="401"/>
+      <c r="C136" s="399"/>
+      <c r="D136" s="399"/>
+      <c r="E136" s="400"/>
       <c r="F136" s="28"/>
       <c r="G136" s="28"/>
     </row>
     <row r="137" spans="1:14">
       <c r="A137" s="30"/>
-      <c r="B137" s="399" t="s">
+      <c r="B137" s="398" t="s">
         <v>453</v>
       </c>
-      <c r="C137" s="401"/>
-      <c r="D137" s="399" t="s">
+      <c r="C137" s="400"/>
+      <c r="D137" s="398" t="s">
         <v>454</v>
       </c>
-      <c r="E137" s="401"/>
+      <c r="E137" s="400"/>
       <c r="F137" s="28"/>
       <c r="G137" s="28"/>
     </row>
@@ -65693,13 +65694,13 @@
       <c r="G163" s="28"/>
     </row>
     <row r="165" spans="1:7">
-      <c r="A165" s="398" t="s">
+      <c r="A165" s="401" t="s">
         <v>183</v>
       </c>
-      <c r="B165" s="398"/>
-      <c r="C165" s="398"/>
-      <c r="D165" s="398"/>
-      <c r="E165" s="398"/>
+      <c r="B165" s="401"/>
+      <c r="C165" s="401"/>
+      <c r="D165" s="401"/>
+      <c r="E165" s="401"/>
     </row>
     <row r="166" spans="1:7" ht="14.65" thickBot="1">
       <c r="A166" s="23" t="s">
@@ -65722,10 +65723,10 @@
       <c r="B168" s="46"/>
     </row>
     <row r="169" spans="1:7">
-      <c r="A169" s="398" t="s">
+      <c r="A169" s="401" t="s">
         <v>443</v>
       </c>
-      <c r="B169" s="398"/>
+      <c r="B169" s="401"/>
     </row>
     <row r="170" spans="1:7">
       <c r="A170" s="23" t="s">
@@ -65757,13 +65758,13 @@
       <c r="B173" s="46"/>
     </row>
     <row r="174" spans="1:7">
-      <c r="A174" s="398" t="s">
+      <c r="A174" s="401" t="s">
         <v>192</v>
       </c>
-      <c r="B174" s="398"/>
-      <c r="C174" s="398"/>
-      <c r="D174" s="398"/>
-      <c r="E174" s="398"/>
+      <c r="B174" s="401"/>
+      <c r="C174" s="401"/>
+      <c r="D174" s="401"/>
+      <c r="E174" s="401"/>
     </row>
     <row r="175" spans="1:7" ht="14.65" thickBot="1">
       <c r="A175" s="23" t="s">
@@ -65783,13 +65784,13 @@
       </c>
     </row>
     <row r="178" spans="1:5">
-      <c r="A178" s="398" t="s">
+      <c r="A178" s="401" t="s">
         <v>186</v>
       </c>
-      <c r="B178" s="398"/>
-      <c r="C178" s="398"/>
-      <c r="D178" s="398"/>
-      <c r="E178" s="398"/>
+      <c r="B178" s="401"/>
+      <c r="C178" s="401"/>
+      <c r="D178" s="401"/>
+      <c r="E178" s="401"/>
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="25" t="s">
@@ -65817,13 +65818,13 @@
       </c>
     </row>
     <row r="183" spans="1:5">
-      <c r="A183" s="398" t="s">
+      <c r="A183" s="401" t="s">
         <v>188</v>
       </c>
-      <c r="B183" s="398"/>
-      <c r="C183" s="398"/>
-      <c r="D183" s="398"/>
-      <c r="E183" s="398"/>
+      <c r="B183" s="401"/>
+      <c r="C183" s="401"/>
+      <c r="D183" s="401"/>
+      <c r="E183" s="401"/>
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="23" t="s">
@@ -65878,13 +65879,13 @@
       </c>
     </row>
     <row r="191" spans="1:5">
-      <c r="A191" s="398" t="s">
+      <c r="A191" s="401" t="s">
         <v>202</v>
       </c>
-      <c r="B191" s="398"/>
-      <c r="C191" s="398"/>
-      <c r="D191" s="398"/>
-      <c r="E191" s="398"/>
+      <c r="B191" s="401"/>
+      <c r="C191" s="401"/>
+      <c r="D191" s="401"/>
+      <c r="E191" s="401"/>
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="21" t="s">
@@ -65944,6 +65945,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -65958,12 +65965,6 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Edit to guidance text for CES
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="10" r:id="rId1"/>
@@ -7486,7 +7486,7 @@
     <t>**Description:** This policy causes the specified quantity of otherwise non-retiring coal capacity to be retired each year. // **Guidance for setting values:** India had 191 GW of coal capacity in 2018, about 43 GW of which is projected to retire by 2027 in the BAU case as per Central Electricity Authority (CEA's) National Electricity Plan. This includes actual retirements till 2019. An additional retirement setting of 7,000 MW/year would retire all of the pre-existing coal capacity by 2032.</t>
   </si>
   <si>
-    <t>**Description:** This policy specifies an increase in the fraction of electricity generation that must come from qualifying carbon-free sources (wind, solar, and biomass) in 2050.  This policy has no effect until the user-set value exceeds the existing fraction of carbon-free electricity and any carbon-free electricity standards which have been enacted at the state level. // **Guidance for setting values:** India's Renewable Purchase Obligations (RPOs) have not been met historically. For this reason, the BAU case does not assume any RPO targets are met. However, the BAU case does assume India meets 80% of its Intended Nationally Determined Contribution for wind and solar.
+    <t>**Description:** This policy specifies an increase in the fraction of electricity generation that must come from qualifying carbon-free sources (wind, solar, and biomass) in 2050.  This policy has no effect until the user-set value exceeds the existing fraction of carbon-free electricity and any carbon-free electricity standards which have been enacted at the state level. // **Guidance for setting values:** India's Renewable Purchase Obligations (RPOs) have not been met historically. For this reason, the BAU case does not assume any RPO targets are met. However, the BAU case does assume India meets 80% of its Nationally Determined Contribution of increasing renewable power capacity to 175 gigawatts by 2022, under the Paris Agreement. 
 If the policy "Expand Carbon-free Electricity Standard Qualifying Definitions" is also enabled, the lever setting is a total RPO target that includes generation from wind, solar, geothermal, and Municipal Solid Waste (MSW) sources. Geothermal and MSW are included as they may be feasible for a more ambitious Renewable Energy (RE) scenario with a delayed start. Biomass is excluded because it has issues such as adverse impacts on local air quality, competing land use, and feedstock availability challenges. Nuclear is excluded because of the need to manage radioactive waste, and hydro is not included due to potential state-level challenges in implementing additional capacity. When setting a high target with the CES lever, users should also turn on supporting power sector policies (i.e., Grid-Scale Electricity Storage, Increase Transmission, and Demand Response) to avoid curtailment of renewables.</t>
   </si>
 </sst>
@@ -9634,9 +9634,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -9645,6 +9642,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -10781,7 +10781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -11031,9 +11031,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T589"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B232" sqref="B232"/>
+    <sheetView topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P178" sqref="P178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -21814,7 +21814,7 @@
       <c r="S177" s="57"/>
       <c r="T177" s="57"/>
     </row>
-    <row r="178" spans="1:20" s="5" customFormat="1" ht="185.25">
+    <row r="178" spans="1:20" s="5" customFormat="1" ht="199.5">
       <c r="A178" s="96" t="s">
         <v>8</v>
       </c>
@@ -64566,13 +64566,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="404" t="s">
+      <c r="A1" s="407" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="404"/>
-      <c r="C1" s="404"/>
-      <c r="D1" s="404"/>
-      <c r="E1" s="404"/>
+      <c r="B1" s="407"/>
+      <c r="C1" s="407"/>
+      <c r="D1" s="407"/>
+      <c r="E1" s="407"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="408" t="s">
@@ -64641,13 +64641,13 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="404" t="s">
+      <c r="A60" s="407" t="s">
         <v>176</v>
       </c>
-      <c r="B60" s="404"/>
-      <c r="C60" s="404"/>
-      <c r="D60" s="404"/>
-      <c r="E60" s="404"/>
+      <c r="B60" s="407"/>
+      <c r="C60" s="407"/>
+      <c r="D60" s="407"/>
+      <c r="E60" s="407"/>
     </row>
     <row r="85" spans="1:39" s="12" customFormat="1">
       <c r="A85" s="9" t="s">
@@ -64752,13 +64752,13 @@
       </c>
     </row>
     <row r="89" spans="1:39">
-      <c r="A89" s="404" t="s">
+      <c r="A89" s="407" t="s">
         <v>177</v>
       </c>
-      <c r="B89" s="404"/>
-      <c r="C89" s="404"/>
-      <c r="D89" s="404"/>
-      <c r="E89" s="404"/>
+      <c r="B89" s="407"/>
+      <c r="C89" s="407"/>
+      <c r="D89" s="407"/>
+      <c r="E89" s="407"/>
     </row>
     <row r="90" spans="1:39">
       <c r="A90" s="9">
@@ -64845,13 +64845,13 @@
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="404" t="s">
+      <c r="A98" s="407" t="s">
         <v>178</v>
       </c>
-      <c r="B98" s="404"/>
-      <c r="C98" s="404"/>
-      <c r="D98" s="404"/>
-      <c r="E98" s="404"/>
+      <c r="B98" s="407"/>
+      <c r="C98" s="407"/>
+      <c r="D98" s="407"/>
+      <c r="E98" s="407"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="17">
@@ -64935,13 +64935,13 @@
       <c r="A108" s="20"/>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="404" t="s">
+      <c r="A109" s="407" t="s">
         <v>180</v>
       </c>
-      <c r="B109" s="404"/>
-      <c r="C109" s="404"/>
-      <c r="D109" s="404"/>
-      <c r="E109" s="404"/>
+      <c r="B109" s="407"/>
+      <c r="C109" s="407"/>
+      <c r="D109" s="407"/>
+      <c r="E109" s="407"/>
     </row>
     <row r="110" spans="1:5" ht="14.65" thickBot="1"/>
     <row r="111" spans="1:5" ht="14.65" thickBot="1">
@@ -64954,13 +64954,13 @@
       </c>
     </row>
     <row r="113" spans="1:14">
-      <c r="A113" s="404" t="s">
+      <c r="A113" s="407" t="s">
         <v>179</v>
       </c>
-      <c r="B113" s="404"/>
-      <c r="C113" s="404"/>
-      <c r="D113" s="404"/>
-      <c r="E113" s="404"/>
+      <c r="B113" s="407"/>
+      <c r="C113" s="407"/>
+      <c r="D113" s="407"/>
+      <c r="E113" s="407"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="17">
@@ -65041,13 +65041,13 @@
       </c>
     </row>
     <row r="124" spans="1:14">
-      <c r="A124" s="404" t="s">
+      <c r="A124" s="407" t="s">
         <v>434</v>
       </c>
-      <c r="B124" s="404"/>
-      <c r="C124" s="404"/>
-      <c r="D124" s="404"/>
-      <c r="E124" s="404"/>
+      <c r="B124" s="407"/>
+      <c r="C124" s="407"/>
+      <c r="D124" s="407"/>
+      <c r="E124" s="407"/>
       <c r="L124" s="21"/>
     </row>
     <row r="125" spans="1:14">
@@ -65138,13 +65138,13 @@
       <c r="C133" s="15"/>
     </row>
     <row r="134" spans="1:14">
-      <c r="A134" s="404" t="s">
+      <c r="A134" s="407" t="s">
         <v>110</v>
       </c>
-      <c r="B134" s="404"/>
-      <c r="C134" s="404"/>
-      <c r="D134" s="404"/>
-      <c r="E134" s="404"/>
+      <c r="B134" s="407"/>
+      <c r="C134" s="407"/>
+      <c r="D134" s="407"/>
+      <c r="E134" s="407"/>
     </row>
     <row r="135" spans="1:14">
       <c r="A135" s="27" t="s">
@@ -65159,25 +65159,25 @@
     </row>
     <row r="136" spans="1:14">
       <c r="A136" s="29"/>
-      <c r="B136" s="405" t="s">
+      <c r="B136" s="404" t="s">
         <v>451</v>
       </c>
-      <c r="C136" s="406"/>
-      <c r="D136" s="406"/>
-      <c r="E136" s="407"/>
+      <c r="C136" s="405"/>
+      <c r="D136" s="405"/>
+      <c r="E136" s="406"/>
       <c r="F136" s="28"/>
       <c r="G136" s="28"/>
     </row>
     <row r="137" spans="1:14">
       <c r="A137" s="30"/>
-      <c r="B137" s="405" t="s">
+      <c r="B137" s="404" t="s">
         <v>452</v>
       </c>
-      <c r="C137" s="407"/>
-      <c r="D137" s="405" t="s">
+      <c r="C137" s="406"/>
+      <c r="D137" s="404" t="s">
         <v>453</v>
       </c>
-      <c r="E137" s="407"/>
+      <c r="E137" s="406"/>
       <c r="F137" s="28"/>
       <c r="G137" s="28"/>
     </row>
@@ -65724,13 +65724,13 @@
       <c r="G163" s="28"/>
     </row>
     <row r="165" spans="1:7">
-      <c r="A165" s="404" t="s">
+      <c r="A165" s="407" t="s">
         <v>183</v>
       </c>
-      <c r="B165" s="404"/>
-      <c r="C165" s="404"/>
-      <c r="D165" s="404"/>
-      <c r="E165" s="404"/>
+      <c r="B165" s="407"/>
+      <c r="C165" s="407"/>
+      <c r="D165" s="407"/>
+      <c r="E165" s="407"/>
     </row>
     <row r="166" spans="1:7" ht="14.65" thickBot="1">
       <c r="A166" s="23" t="s">
@@ -65753,10 +65753,10 @@
       <c r="B168" s="46"/>
     </row>
     <row r="169" spans="1:7">
-      <c r="A169" s="404" t="s">
+      <c r="A169" s="407" t="s">
         <v>442</v>
       </c>
-      <c r="B169" s="404"/>
+      <c r="B169" s="407"/>
     </row>
     <row r="170" spans="1:7">
       <c r="A170" s="23" t="s">
@@ -65788,13 +65788,13 @@
       <c r="B173" s="46"/>
     </row>
     <row r="174" spans="1:7">
-      <c r="A174" s="404" t="s">
+      <c r="A174" s="407" t="s">
         <v>192</v>
       </c>
-      <c r="B174" s="404"/>
-      <c r="C174" s="404"/>
-      <c r="D174" s="404"/>
-      <c r="E174" s="404"/>
+      <c r="B174" s="407"/>
+      <c r="C174" s="407"/>
+      <c r="D174" s="407"/>
+      <c r="E174" s="407"/>
     </row>
     <row r="175" spans="1:7" ht="14.65" thickBot="1">
       <c r="A175" s="23" t="s">
@@ -65814,13 +65814,13 @@
       </c>
     </row>
     <row r="178" spans="1:5">
-      <c r="A178" s="404" t="s">
+      <c r="A178" s="407" t="s">
         <v>186</v>
       </c>
-      <c r="B178" s="404"/>
-      <c r="C178" s="404"/>
-      <c r="D178" s="404"/>
-      <c r="E178" s="404"/>
+      <c r="B178" s="407"/>
+      <c r="C178" s="407"/>
+      <c r="D178" s="407"/>
+      <c r="E178" s="407"/>
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="25" t="s">
@@ -65848,13 +65848,13 @@
       </c>
     </row>
     <row r="183" spans="1:5">
-      <c r="A183" s="404" t="s">
+      <c r="A183" s="407" t="s">
         <v>188</v>
       </c>
-      <c r="B183" s="404"/>
-      <c r="C183" s="404"/>
-      <c r="D183" s="404"/>
-      <c r="E183" s="404"/>
+      <c r="B183" s="407"/>
+      <c r="C183" s="407"/>
+      <c r="D183" s="407"/>
+      <c r="E183" s="407"/>
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="23" t="s">
@@ -65909,13 +65909,13 @@
       </c>
     </row>
     <row r="191" spans="1:5">
-      <c r="A191" s="404" t="s">
+      <c r="A191" s="407" t="s">
         <v>202</v>
       </c>
-      <c r="B191" s="404"/>
-      <c r="C191" s="404"/>
-      <c r="D191" s="404"/>
-      <c r="E191" s="404"/>
+      <c r="B191" s="407"/>
+      <c r="C191" s="407"/>
+      <c r="D191" s="407"/>
+      <c r="E191" s="407"/>
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="21" t="s">
@@ -65975,6 +65975,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -65989,12 +65995,6 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>